<commit_message>
Fix BE language support
</commit_message>
<xml_diff>
--- a/src/info/species/data/species.xlsx
+++ b/src/info/species/data/species.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Base" sheetId="1" state="visible" r:id="rId2"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:v2="http://schemas.openxmlformats.org/spreadsheetml/2006/main/v2" mc:Ignorable="v2">
   <authors>
     <author/>
   </authors>
@@ -61,6 +61,27 @@
           <t xml:space="preserve">I would leave it in English</t>
         </r>
       </text>
+      <mc:AlternateContent>
+        <mc:Choice Requires="v2">
+          <commentPr autoFill="true" autoScale="false" colHidden="false" locked="false" rowHidden="false" textHAlign="justify" textVAlign="justify">
+            <anchor moveWithCells="false" sizeWithCells="false">
+              <xdr:from>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>16</xdr:colOff>
+                <xdr:row>126</xdr:row>
+                <xdr:rowOff>7</xdr:rowOff>
+              </xdr:from>
+              <xdr:to>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>88</xdr:colOff>
+                <xdr:row>127</xdr:row>
+                <xdr:rowOff>48</xdr:rowOff>
+              </xdr:to>
+            </anchor>
+          </commentPr>
+        </mc:Choice>
+        <mc:Fallback/>
+      </mc:AlternateContent>
     </comment>
     <comment ref="J113" authorId="0">
       <text>
@@ -87,6 +108,27 @@
           <t xml:space="preserve">so the name of the project will be Ladybird Survey? Shall we translate it into each language? I suggest not but please let me know (I've generally translated it as progetto di ricerca sulle coccinelle)</t>
         </r>
       </text>
+      <mc:AlternateContent>
+        <mc:Choice Requires="v2">
+          <commentPr autoFill="true" autoScale="false" colHidden="false" locked="false" rowHidden="false" textHAlign="justify" textVAlign="justify">
+            <anchor moveWithCells="false" sizeWithCells="false">
+              <xdr:from>
+                <xdr:col>10</xdr:col>
+                <xdr:colOff>35</xdr:colOff>
+                <xdr:row>110</xdr:row>
+                <xdr:rowOff>65</xdr:rowOff>
+              </xdr:from>
+              <xdr:to>
+                <xdr:col>11</xdr:col>
+                <xdr:colOff>107</xdr:colOff>
+                <xdr:row>111</xdr:row>
+                <xdr:rowOff>113</xdr:rowOff>
+              </xdr:to>
+            </anchor>
+          </commentPr>
+        </mc:Choice>
+        <mc:Fallback/>
+      </mc:AlternateContent>
     </comment>
     <comment ref="J130" authorId="0">
       <text>
@@ -113,6 +155,27 @@
           <t xml:space="preserve">I've put it as plural, since it is so reported in English</t>
         </r>
       </text>
+      <mc:AlternateContent>
+        <mc:Choice Requires="v2">
+          <commentPr autoFill="true" autoScale="false" colHidden="false" locked="false" rowHidden="false" textHAlign="justify" textVAlign="justify">
+            <anchor moveWithCells="false" sizeWithCells="false">
+              <xdr:from>
+                <xdr:col>10</xdr:col>
+                <xdr:colOff>16</xdr:colOff>
+                <xdr:row>126</xdr:row>
+                <xdr:rowOff>7</xdr:rowOff>
+              </xdr:from>
+              <xdr:to>
+                <xdr:col>11</xdr:col>
+                <xdr:colOff>88</xdr:colOff>
+                <xdr:row>127</xdr:row>
+                <xdr:rowOff>48</xdr:rowOff>
+              </xdr:to>
+            </anchor>
+          </commentPr>
+        </mc:Choice>
+        <mc:Fallback/>
+      </mc:AlternateContent>
     </comment>
   </commentList>
 </comments>
@@ -307,10 +370,10 @@
     <t xml:space="preserve">BE {order}</t>
   </si>
   <si>
-    <t xml:space="preserve">BE {common_name { NL }}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BE {common_name { FR }}</t>
+    <t xml:space="preserve">BE {common_name {NL}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BE {common_name {FR}}</t>
   </si>
   <si>
     <t xml:space="preserve">BE {habitat {comment[]}}</t>
@@ -328,10 +391,10 @@
     <t xml:space="preserve">BE {comment_EN}</t>
   </si>
   <si>
-    <t xml:space="preserve">BE {comment { NL }}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BE {comment { FR }}</t>
+    <t xml:space="preserve">BE {comment {NL}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BE {comment {FR}}</t>
   </si>
   <si>
     <t xml:space="preserve">?</t>
@@ -14447,12 +14510,12 @@
   </sheetPr>
   <dimension ref="A1:AMJ73"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="BM70" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="DK2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="BM1" activeCellId="0" sqref="BM1"/>
-      <selection pane="bottomLeft" activeCell="A70" activeCellId="0" sqref="A70"/>
-      <selection pane="bottomRight" activeCell="BX56" activeCellId="0" sqref="BX56"/>
+      <selection pane="topRight" activeCell="DK1" activeCellId="0" sqref="DK1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="DM2" activeCellId="0" sqref="DM2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14520,7 +14583,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="160" style="0" width="8.86"/>
   </cols>
   <sheetData>
-    <row r="1" s="22" customFormat="true" ht="63.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="22" customFormat="true" ht="161.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -48315,8 +48378,8 @@
   </sheetPr>
   <dimension ref="A1:GA135"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="EA124" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="EQ127" activeCellId="0" sqref="EQ127"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A29" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D178" activeCellId="0" sqref="D178"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Move photos out of spreadsheet
</commit_message>
<xml_diff>
--- a/src/info/species/data/species.xlsx
+++ b/src/info/species/data/species.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10210"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -9,19 +9,17 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14240" tabRatio="808" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20" yWindow="0" windowWidth="28800" windowHeight="14240" tabRatio="808"/>
   </bookViews>
   <sheets>
     <sheet name="Base" sheetId="1" r:id="rId1"/>
     <sheet name="Species" sheetId="2" r:id="rId2"/>
     <sheet name="Charact_default" sheetId="3" r:id="rId3"/>
     <sheet name="Characteristics_overview" sheetId="4" r:id="rId4"/>
-    <sheet name="Photos" sheetId="6" r:id="rId5"/>
-    <sheet name="Photos - additions" sheetId="7" r:id="rId6"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId7"/>
-    <externalReference r:id="rId8"/>
+    <externalReference r:id="rId5"/>
+    <externalReference r:id="rId6"/>
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Base!$C$1:$FC$73</definedName>
@@ -32,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5762" uniqueCount="1113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5492" uniqueCount="1074">
   <si>
     <t>id</t>
   </si>
@@ -3992,123 +3990,6 @@
     <t>Pronotum</t>
   </si>
   <si>
-    <t>width[]</t>
-  </si>
-  <si>
-    <t>height[]</t>
-  </si>
-  <si>
-    <t>author[]</t>
-  </si>
-  <si>
-    <t>Michael Majerus</t>
-  </si>
-  <si>
-    <t>Lindsay Bowes</t>
-  </si>
-  <si>
-    <t>Gilles San Martins</t>
-  </si>
-  <si>
-    <t>APP</t>
-  </si>
-  <si>
-    <t>David Benham</t>
-  </si>
-  <si>
-    <t>Stephen Barlow</t>
-  </si>
-  <si>
-    <t>Philip Appleyard</t>
-  </si>
-  <si>
-    <t>Peter Brown</t>
-  </si>
-  <si>
-    <t>Maris Midgley</t>
-  </si>
-  <si>
-    <t>Richard Comont</t>
-  </si>
-  <si>
-    <t>Bruce Martin</t>
-  </si>
-  <si>
-    <t>Michael Kilner</t>
-  </si>
-  <si>
-    <t>Ignacio Alonso</t>
-  </si>
-  <si>
-    <t>Helen Roy</t>
-  </si>
-  <si>
-    <t>Roger Wilson</t>
-  </si>
-  <si>
-    <t>Remy Poland</t>
-  </si>
-  <si>
-    <t>Claire Watson</t>
-  </si>
-  <si>
-    <t>Anne Sorbes</t>
-  </si>
-  <si>
-    <t>Handy</t>
-  </si>
-  <si>
-    <t>Koenraad Bracke</t>
-  </si>
-  <si>
-    <t>Ken Dolbear</t>
-  </si>
-  <si>
-    <t>Paul Brothers</t>
-  </si>
-  <si>
-    <t>Miroslav Fiala</t>
-  </si>
-  <si>
-    <t>Stanislav Krejčík</t>
-  </si>
-  <si>
-    <t>Edward Bartoszewicz</t>
-  </si>
-  <si>
-    <t>Toni Watt</t>
-  </si>
-  <si>
-    <t>Alby Oakshott</t>
-  </si>
-  <si>
-    <t>Josef Dvořák</t>
-  </si>
-  <si>
-    <t>Oldřich Nedvěd</t>
-  </si>
-  <si>
-    <t>Jelena Pincta</t>
-  </si>
-  <si>
-    <t>Jiří Skuhrovec</t>
-  </si>
-  <si>
-    <t>Andgelo Mombert</t>
-  </si>
-  <si>
-    <t>H. Bouyon</t>
-  </si>
-  <si>
-    <t>Nicola Bormolini</t>
-  </si>
-  <si>
-    <t>Saulo Bambi</t>
-  </si>
-  <si>
-    <t>ADD PHOTOS</t>
-  </si>
-  <si>
     <t>Arable land, garden or park</t>
   </si>
   <si>
@@ -4151,7 +4032,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -4535,7 +4416,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="178">
+  <cellXfs count="175">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -5056,11 +4937,6 @@
     <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -5068,7 +4944,7 @@
   <cellStyles count="3">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normale 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Normale 2" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -5476,11 +5352,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMJ73"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="S38" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="S2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="DK1" sqref="DK1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="D39" sqref="D39"/>
@@ -5781,70 +5657,70 @@
         <v>41</v>
       </c>
       <c r="BY1" s="9" t="s">
-        <v>1103</v>
+        <v>1064</v>
       </c>
       <c r="BZ1" s="7" t="s">
-        <v>1104</v>
+        <v>1065</v>
       </c>
       <c r="CA1" s="7" t="s">
-        <v>1105</v>
+        <v>1066</v>
       </c>
       <c r="CB1" s="10" t="s">
-        <v>1106</v>
+        <v>1067</v>
       </c>
       <c r="CC1" s="10" t="s">
-        <v>1106</v>
+        <v>1067</v>
       </c>
       <c r="CD1" s="10" t="s">
-        <v>1106</v>
+        <v>1067</v>
       </c>
       <c r="CE1" s="11" t="s">
-        <v>1107</v>
+        <v>1068</v>
       </c>
       <c r="CF1" s="11" t="s">
-        <v>1107</v>
+        <v>1068</v>
       </c>
       <c r="CG1" s="11" t="s">
-        <v>1107</v>
+        <v>1068</v>
       </c>
       <c r="CH1" s="11" t="s">
-        <v>1107</v>
+        <v>1068</v>
       </c>
       <c r="CI1" s="11" t="s">
-        <v>1107</v>
+        <v>1068</v>
       </c>
       <c r="CJ1" s="11" t="s">
-        <v>1107</v>
+        <v>1068</v>
       </c>
       <c r="CK1" s="11" t="s">
-        <v>1107</v>
+        <v>1068</v>
       </c>
       <c r="CL1" s="11" t="s">
-        <v>1107</v>
+        <v>1068</v>
       </c>
       <c r="CM1" s="11" t="s">
-        <v>1107</v>
+        <v>1068</v>
       </c>
       <c r="CN1" s="11" t="s">
-        <v>1107</v>
+        <v>1068</v>
       </c>
       <c r="CO1" s="10" t="s">
-        <v>1108</v>
+        <v>1069</v>
       </c>
       <c r="CP1" s="10" t="s">
-        <v>1108</v>
+        <v>1069</v>
       </c>
       <c r="CQ1" s="10" t="s">
-        <v>1108</v>
+        <v>1069</v>
       </c>
       <c r="CR1" s="7" t="s">
-        <v>1109</v>
+        <v>1070</v>
       </c>
       <c r="CS1" s="13" t="s">
-        <v>1110</v>
+        <v>1071</v>
       </c>
       <c r="CT1" s="12" t="s">
-        <v>1111</v>
+        <v>1072</v>
       </c>
       <c r="CU1" s="9" t="s">
         <v>42</v>
@@ -11626,7 +11502,7 @@
         <v>16</v>
       </c>
       <c r="AB20" s="51" t="s">
-        <v>1102</v>
+        <v>1063</v>
       </c>
       <c r="AC20" s="34" t="s">
         <v>85</v>
@@ -20782,7 +20658,7 @@
         <v>35</v>
       </c>
       <c r="AB40" s="31" t="s">
-        <v>1112</v>
+        <v>1073</v>
       </c>
       <c r="AC40" s="34" t="s">
         <v>529</v>
@@ -33005,9 +32881,9 @@
       <c r="FC73" s="142"/>
     </row>
   </sheetData>
-  <autoFilter ref="C1:FC73" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="C1:FC73"/>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" sqref="AQ2:AQ18 AQ20:AQ44" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" sqref="AQ2:AQ18 AQ20:AQ44">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -33017,7 +32893,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="118">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$H$2:$H$11</xm:f>
           </x14:formula1>
@@ -33026,7 +32902,7 @@
           </x14:formula2>
           <xm:sqref>T2 T68:T73</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000002000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$I$2:$I$9</xm:f>
           </x14:formula1>
@@ -33035,7 +32911,7 @@
           </x14:formula2>
           <xm:sqref>U2:U23 Q24:Q25 U26:U29 Q27:Q28 U30:U45 U48:U50 U52:U57 U59:U61 U64:U73</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000003000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$J$2:$J$21</xm:f>
           </x14:formula1>
@@ -33044,7 +32920,7 @@
           </x14:formula2>
           <xm:sqref>Q2:Q7 Q9:Q23 Q26 Q29:Q42 Q45 Q66:Q69 Q71 Q73</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000004000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$L$2:$L$27</xm:f>
           </x14:formula1>
@@ -33053,7 +32929,7 @@
           </x14:formula2>
           <xm:sqref>AC2:AE2 AR2:AT2 BJ2:BL2 CB2:CD2 DU2:DW2 EZ2 DU3:DU4 AC66:AI73 AR66:AT73 BP66:BP73 CP66:CP67 DL66:DL71 EI66:EI69 EZ66:EZ73 EI71:EI73 DL73</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000005000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$M$2:$M$24</xm:f>
           </x14:formula1>
@@ -33062,7 +32938,7 @@
           </x14:formula2>
           <xm:sqref>AK2:AL2 BA2:BC2 BS2:BU2 CO2:CQ4 DL2:DM6 EH2:EJ4 FA2 BB3:BC14 BT3:BU14 CP5:CQ14 EI5:EJ9 DM7:DM8 DL9:DM9 EJ10 DM11:DM13 EI11:EJ13 DL14:DM14 BC15 BU15 CQ15 DM15 BB16:BC16 BT16:BU16 CP16:CQ16 DL16:DM16 DL17:DL23 EI21:EJ23 DL24:DM36 EI29:EJ36 EI38:EJ38 DL39:DM40 EI41:EJ44 AJ66:AL71 BA66:BC73 BQ66:BS73 CQ66:CQ67 DM66:DM71 EJ66:EJ73 FA66:FA73 EI70:EJ70 AJ72:AL73 DM73</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000006000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$O$2:$O$12</xm:f>
           </x14:formula1>
@@ -33071,7 +32947,7 @@
           </x14:formula2>
           <xm:sqref>W2:Y2 X3:Y9 Y10:Y40 X41:Y44 X46 W50:W53 W55:W56 W58 W60:W65 X65 X66:Y68 W68:Y68 W69 Y69:Y70 X70:Y70 W71:W72 X72:Y73</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000007000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$M$2:$M$27</xm:f>
           </x14:formula1>
@@ -33080,7 +32956,7 @@
           </x14:formula2>
           <xm:sqref>AJ45:AL45 BA45:BC45 BS45:BU45 CO45:CQ45 DM45 EJ45 FA45</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000008000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$O$2:$O$13</xm:f>
           </x14:formula1>
@@ -33089,7 +32965,7 @@
           </x14:formula2>
           <xm:sqref>W45:Y45 W46 Y46:Y48 X47:Y47 Y50:Y64 X51:Y54 X56:Y60 X62:Y63 W70 X71:Y71</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000009000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$M$2:$M$28</xm:f>
           </x14:formula1>
@@ -33098,7 +32974,7 @@
           </x14:formula2>
           <xm:sqref>AJ46:AL46 BA46:BC46 BS46:BU46 CQ46 DM46 EJ46 FA46</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-00000A000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$L$2:$L$30</xm:f>
           </x14:formula1>
@@ -33107,7 +32983,7 @@
           </x14:formula2>
           <xm:sqref>AT45:AT50 BL45:BL50 AC47:AI48 AR47:AT48 BJ47:BL48 CB47:CD48 DL47:DL48 EI47:EI48 EZ47:EZ48 CP48 CC49:CD50 AC50:AI50 AS50:AT50 BK50:BL50 CY50 EI50 EZ50 AT52:AT54 BL52:BL54 CD52:CD53 CZ52:CZ53 AS54:AT54 BK54:BL54 CD55 CZ55 DV55:DW55 AT56:AT59 BL56:BL59 CC56:CD57 AS57:AT57 BK57:BL57 DV57:DW57 AC58:AI58 DL58 EI58 EZ58 CD59 CZ59 AT61 BL61 CC61:CD62 CY61:CZ61 DU61:DU62 AC62:AI62 AS62:AT63 BK62:BL64 DL62 EI62 EZ62 AS64:AT64 DV64:DW64 AT65 BL65 CD65 CZ65</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-00000B000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$M$2:$M$29</xm:f>
           </x14:formula1>
@@ -33116,7 +32992,7 @@
           </x14:formula2>
           <xm:sqref>CQ20 EJ20 AM46 CR46 DN46:DO46 EK46:EN46 FB46 AJ47:AL47 BA47:BC47 BT47:BU47 DM47 EJ47 FA47 BU48 BB54 BT54 BB55:BC58 BT55:BU58 CP55:CQ59 AJ56:AL56 BA56:BC56 BS56:BU56 CO56:CQ56 DM56 EJ56 FA56 AJ58:AL58 DM58 EJ58 FA58 BC59 BU59 BB60:BC60 BT60:BU60 EI60:EJ60 BC61 BU61 AJ62:AL62 BA62:BC62 BS62:BU62 CO62:CQ62 DM62 EJ62 FA62 BA63 BS63 CO63 CQ63:CQ64 DK63 BC64 BU64 DM64 EJ64</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-00000C000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$J$2:$J$40</xm:f>
           </x14:formula1>
@@ -33125,7 +33001,7 @@
           </x14:formula2>
           <xm:sqref>Q47:Q48</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-00000D000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$O$2:$O$14</xm:f>
           </x14:formula1>
@@ -33134,7 +33010,7 @@
           </x14:formula2>
           <xm:sqref>X55</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-00000E000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$M$2:$M$47</xm:f>
           </x14:formula1>
@@ -33143,7 +33019,7 @@
           </x14:formula2>
           <xm:sqref>CP47:CQ47 AJ48:AL48 BA48:BB48 BS48:BT48 CQ48 DM48 EJ48 FA48</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-00000F000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$L$2:$L$31</xm:f>
           </x14:formula1>
@@ -33152,7 +33028,7 @@
           </x14:formula2>
           <xm:sqref>AC49:AI49 AR49 BJ49 CB49:CB50 CX49 EZ49</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000010000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$M$2:$M$32</xm:f>
           </x14:formula1>
@@ -33161,7 +33037,7 @@
           </x14:formula2>
           <xm:sqref>AJ49:AL49 BA49:BC49 BS49:BU49 CO49:CQ49 EH49:EJ49 FA49 AJ63:AL63 BC63 BU63 CP63 DL63 EJ63 FA63</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000011000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$O$2:$O$16</xm:f>
           </x14:formula1>
@@ -33170,7 +33046,7 @@
           </x14:formula2>
           <xm:sqref>W49:Y49 X64</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000012000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$M$2:$M$34</xm:f>
           </x14:formula1>
@@ -33179,7 +33055,7 @@
           </x14:formula2>
           <xm:sqref>BC48:BD48 AJ50:AL50 BA50:BC50 BS50:BU50 CO50:CQ50 EJ50 FA50 BC52:BC53 BU52:BU54 CQ52 BC54</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000013000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$M$2:$M$35</xm:f>
           </x14:formula1>
@@ -33188,7 +33064,7 @@
           </x14:formula2>
           <xm:sqref>AJ52:AL52 BB52 BT52 CP52 EJ52 FA52</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000014000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$M$2:$M$36</xm:f>
           </x14:formula1>
@@ -33197,7 +33073,7 @@
           </x14:formula2>
           <xm:sqref>AJ51:AL51 BA51 BS51 CQ51 DM51 EJ51 FA51 AJ53:AL53 BB53 BT53 CP53 DM53:DM54 EJ53 FA53 AC54:AL54 AR54 BA54 BJ54 BS54 CP54:CQ54 EI54:EJ54 EZ54:FA54 CQ68:CQ69</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000015000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$J$2:$J$25</xm:f>
           </x14:formula1>
@@ -33206,7 +33082,7 @@
           </x14:formula2>
           <xm:sqref>Q54</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000016000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$O$2:$O$17</xm:f>
           </x14:formula1>
@@ -33215,7 +33091,7 @@
           </x14:formula2>
           <xm:sqref>W3:W44 X61 W66:W67 W73</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000017000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$J$2:$J$26</xm:f>
           </x14:formula1>
@@ -33224,7 +33100,7 @@
           </x14:formula2>
           <xm:sqref>Q8 Q55</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000018000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$L$2:$L$38</xm:f>
           </x14:formula1>
@@ -33233,7 +33109,7 @@
           </x14:formula2>
           <xm:sqref>AC55:AI55 AR55 BJ55 CX55 EI55 EZ55</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000019000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$M$2:$M$37</xm:f>
           </x14:formula1>
@@ -33242,7 +33118,7 @@
           </x14:formula2>
           <xm:sqref>AJ55:AL55 BA55 BS55 CO55 DM55 EJ55 FA55</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-00001A000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$J$2:$J$27</xm:f>
           </x14:formula1>
@@ -33251,7 +33127,7 @@
           </x14:formula2>
           <xm:sqref>Q57</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-00001B000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$M$2:$M$38</xm:f>
           </x14:formula1>
@@ -33260,7 +33136,7 @@
           </x14:formula2>
           <xm:sqref>AJ57:AL57 BA57 BS57 DM57 EJ57 FA57</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-00001C000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$J$2:$J$28</xm:f>
           </x14:formula1>
@@ -33269,7 +33145,7 @@
           </x14:formula2>
           <xm:sqref>Q58</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-00001D000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$J$2:$J$29</xm:f>
           </x14:formula1>
@@ -33278,7 +33154,7 @@
           </x14:formula2>
           <xm:sqref>Q59</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-00001E000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$L$2:$L$41</xm:f>
           </x14:formula1>
@@ -33287,7 +33163,7 @@
           </x14:formula2>
           <xm:sqref>AC59:AI59 AR59 BJ59 CB59 CX59 DL59 EI59 EZ59</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-00001F000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$M$2:$M$40</xm:f>
           </x14:formula1>
@@ -33296,7 +33172,7 @@
           </x14:formula2>
           <xm:sqref>CO57 AJ59:AL61 BA59:BB59 BS59:BT59 CO59 DM59:DM60 EJ59 FA59:FA61 CQ60 EH60 BA61 BS61 CO61 EJ61</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000020000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$J$2:$J$30</xm:f>
           </x14:formula1>
@@ -33305,7 +33181,7 @@
           </x14:formula2>
           <xm:sqref>Q60</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000021000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$L$2:$L$43</xm:f>
           </x14:formula1>
@@ -33314,7 +33190,7 @@
           </x14:formula2>
           <xm:sqref>AC60:AI60 AR60:AT60 BJ60:BL60 CB60:CD60 CP60 DL60 DU60 EZ60 CB61:CB64 CX61 CX63:CX64 CC64:CD64 CY64:CZ64 CB66:CB68</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000022000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$J$2:$J$31</xm:f>
           </x14:formula1>
@@ -33323,7 +33199,7 @@
           </x14:formula2>
           <xm:sqref>Q61</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000023000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$M$2:$M$41</xm:f>
           </x14:formula1>
@@ -33332,7 +33208,7 @@
           </x14:formula2>
           <xm:sqref>BB61 BT61 CP61 DK61 AJ64:AL65 FA64:FA65 EJ65</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000024000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$J$2:$J$32</xm:f>
           </x14:formula1>
@@ -33341,7 +33217,7 @@
           </x14:formula2>
           <xm:sqref>Q62</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000025000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$J$2:$J$33</xm:f>
           </x14:formula1>
@@ -33350,7 +33226,7 @@
           </x14:formula2>
           <xm:sqref>Q63</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000026000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$L$2:$L$45</xm:f>
           </x14:formula1>
@@ -33359,7 +33235,7 @@
           </x14:formula2>
           <xm:sqref>AC63:AI63 EI63 EZ63</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000027000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$J$2:$J$35</xm:f>
           </x14:formula1>
@@ -33368,7 +33244,7 @@
           </x14:formula2>
           <xm:sqref>Q64</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000028000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$J$2:$J$36</xm:f>
           </x14:formula1>
@@ -33377,7 +33253,7 @@
           </x14:formula2>
           <xm:sqref>Q65</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000029000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$M$2:$M$43</xm:f>
           </x14:formula1>
@@ -33386,7 +33262,7 @@
           </x14:formula2>
           <xm:sqref>BB65:BC65 BT65:BU65 CP65:CQ65 DM65</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-00002A000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$J$2:$J$37</xm:f>
           </x14:formula1>
@@ -33395,7 +33271,7 @@
           </x14:formula2>
           <xm:sqref>Q56</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-00002B000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$J$2:$J$38</xm:f>
           </x14:formula1>
@@ -33404,7 +33280,7 @@
           </x14:formula2>
           <xm:sqref>Q51</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-00002C000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$M$2:$M$45</xm:f>
           </x14:formula1>
@@ -33413,7 +33289,7 @@
           </x14:formula2>
           <xm:sqref>DK2:DK6 AK3:AL13 BA3:BA19 BS3:BS19 FA3:FA44 AJ5:AL13 CO5:CO19 EH5:EH8 DK9 EH10:EH19 AJ14:AJ19 AL14:AL15 DK14:DK16 EJ14 EI15:EJ19 AK16:AL19 BB17:BC19 BT17:BU19 CP17:CQ19 AK20 BB20 BT20 AJ21:AL23 BA21:BC23 BS21:BU23 CO21:CQ23 DK21:DK28 EH21:EH23 AK24:AK28 BB24:BB28 BT24:BT28 CP24:CP28 EI24:EI28 AJ29:AL37 BA29:BC37 BS29:BU37 CO29:CQ37 EH29:EH44 DK30:DK37 DL37:DM37 EI37:EJ37 AJ38:AJ44 BA38:BA44 BS38:BS44 CO38:CO44 DM38 AL39 BC39 BU39 CQ39 DK39 EJ39 AK40:AL44 BB40:BC44 BT40:BU44 CP40:CQ44 EI40:EJ40 DK41:DM44 CO47:CO48 DM49:DM50 BB51:BC51 BT51:BU51 CO51:CO53 BA52:BA53 BS52:BS53 DM52 BB63 BT63 CO68:CO71 CP70:CQ73 EH70 DL72:DM72 CO73:CQ73</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-00002D000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$H$2:$H$12</xm:f>
           </x14:formula1>
@@ -33422,7 +33298,7 @@
           </x14:formula2>
           <xm:sqref>T3:T45 T48:T57 T59:T67</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-00002E000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$J$2:$J$39</xm:f>
           </x14:formula1>
@@ -33431,7 +33307,7 @@
           </x14:formula2>
           <xm:sqref>Q46</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-00002F000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$O$2:$O$19</xm:f>
           </x14:formula1>
@@ -33440,7 +33316,7 @@
           </x14:formula2>
           <xm:sqref>W48:X48</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000030000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$J$2:$J$42</xm:f>
           </x14:formula1>
@@ -33449,7 +33325,7 @@
           </x14:formula2>
           <xm:sqref>Q49:Q50</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000031000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$L$2:$L$53</xm:f>
           </x14:formula1>
@@ -33458,7 +33334,7 @@
           </x14:formula2>
           <xm:sqref>AC52:AI52 EI52 EZ52</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000032000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$O$2:$O$20</xm:f>
           </x14:formula1>
@@ -33467,7 +33343,7 @@
           </x14:formula2>
           <xm:sqref>X50</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000033000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$H$2:$H$13</xm:f>
           </x14:formula1>
@@ -33476,7 +33352,7 @@
           </x14:formula2>
           <xm:sqref>T46:T47 T58</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000034000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$I$2:$I$10</xm:f>
           </x14:formula1>
@@ -33485,7 +33361,7 @@
           </x14:formula2>
           <xm:sqref>U46:U47 U51 U58 U62:U63</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000035000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$J$2:$J$43</xm:f>
           </x14:formula1>
@@ -33494,7 +33370,7 @@
           </x14:formula2>
           <xm:sqref>Q52:Q53</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000036000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$O$2:$O$21</xm:f>
           </x14:formula1>
@@ -33503,7 +33379,7 @@
           </x14:formula2>
           <xm:sqref>W54</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000037000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$L$2:$L$55</xm:f>
           </x14:formula1>
@@ -33512,7 +33388,7 @@
           </x14:formula2>
           <xm:sqref>AC56:AI56 AR56 BJ56 DL56 EI56 EZ56</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000038000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$O$2:$O$22</xm:f>
           </x14:formula1>
@@ -33521,7 +33397,7 @@
           </x14:formula2>
           <xm:sqref>W57</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000039000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$O$2:$O$23</xm:f>
           </x14:formula1>
@@ -33530,7 +33406,7 @@
           </x14:formula2>
           <xm:sqref>Y65</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-00003A000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$L$2:$L$56</xm:f>
           </x14:formula1>
@@ -33539,7 +33415,7 @@
           </x14:formula2>
           <xm:sqref>AC61:AI61 AR61 BJ61 EI61 EZ61</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-00003B000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$L$2:$L$57</xm:f>
           </x14:formula1>
@@ -33548,7 +33424,7 @@
           </x14:formula2>
           <xm:sqref>AS45:AS46 BK45:BK46 CC45:CD45 CC46 AS49 BK49 CY49 AS51:AS52 BK51:BK52 CC51:CC52 CY52 AS55:AS56 BK55:BK56 CB55:CB56 CY55 CB57 AS58:AS59 BK58:BK59 CC59 CY59 AS65 BK65 CC65 CY65 DV65:DW65</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-00003C000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$O$2:$O$24</xm:f>
           </x14:formula1>
@@ -33557,7 +33433,7 @@
           </x14:formula2>
           <xm:sqref>W59</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-00003D000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$M$2:$M$48</xm:f>
           </x14:formula1>
@@ -33566,7 +33442,7 @@
           </x14:formula2>
           <xm:sqref>AJ2:AJ4 AK14 EI14 CO20:CP20 EH20:EI20 BA64:BB64 BS64:BT64 CO64:CP64 DK64:DL64 EH64:EI64 BA65 BS65 CO65 DK65</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-00003E000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$L$2:$L$29</xm:f>
           </x14:formula1>
@@ -33575,7 +33451,7 @@
           </x14:formula2>
           <xm:sqref>AC46:AI46 AR46 BJ46 CB46 CP46 DL46 EI46 EZ46</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-00003F000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$L$2:$L$34</xm:f>
           </x14:formula1>
@@ -33584,7 +33460,7 @@
           </x14:formula2>
           <xm:sqref>AC53:AI53 AR53 BJ53 CB53 CX53 EI53 EZ53</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000040000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$L$2:$L$39</xm:f>
           </x14:formula1>
@@ -33593,7 +33469,7 @@
           </x14:formula2>
           <xm:sqref>DU55 AC57:AI57 AR57 BJ57 DL57 DU57 EI57 EZ57</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000041000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$L$2:$L$50</xm:f>
           </x14:formula1>
@@ -33602,7 +33478,7 @@
           </x14:formula2>
           <xm:sqref>AC3:AE19 AR3:AT15 BJ3:BL15 CB3:CD19 DV3:DW5 EZ3:EZ44 CX6 DU6:DU15 DW6 DV7:DW15 CX14:CZ15 AR16:AR38 AT16 BJ16:BJ38 BL16 CX16 DW16 AS17:AT19 BK17:BL19 DU17:DW19 CX19:CZ19 AC20:AC24 AE20 AT20 BL20 CB20:CB38 CD20:CD22 CX20 CZ20 DU20:DU38 DW20:DW21 AD21:AE44 AS21:AT23 BK21:BL23 CC21:CD28 DV21:DW23 AC25:AE38 AA27:AA28 CD29 CX29:CX44 CC30:CD37 DV32:DW32 DV37:DW37 CY38 AC40:AE44 AR40:AR44 BJ40:BJ44 CB40:CB44 DU40:DU44 AC51:AI51 AR51:AR52 BJ51:BJ52 CB51:CB52 CP51 DL51 EI51 EZ51 CX52 CC66:CC67 CP68:CP69 CB69:CB71 DU70 CB72:CD73 CX72:CZ72</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000042000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$L$2:$L$51</xm:f>
           </x14:formula1>
@@ -33611,7 +33487,7 @@
           </x14:formula2>
           <xm:sqref>AC45:AI45 AR45 BJ45 CB45 DL45 EI45 EZ45</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000043000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Characteristics_overview!$B$1:$J$1</xm:f>
           </x14:formula1>
@@ -33620,7 +33496,7 @@
           </x14:formula2>
           <xm:sqref>E2:H73</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000044000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$L$2:$L$48</xm:f>
           </x14:formula1>
@@ -33629,7 +33505,7 @@
           </x14:formula2>
           <xm:sqref>AC64:AI65 AR64:AR65 BJ64:BJ65 DU64:DU65 EZ64:EZ65 CB65 CX65 EI65</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000045000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$L$2:$L$58</xm:f>
           </x14:formula1>
@@ -33638,7 +33514,7 @@
           </x14:formula2>
           <xm:sqref>AR58 BJ58</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000046000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$L$2:$L$61</xm:f>
           </x14:formula1>
@@ -33647,7 +33523,7 @@
           </x14:formula2>
           <xm:sqref>AR50 BJ50 CX50 AR62:AR63 BJ62:BJ63</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000047000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Characteristics_overview!$B$15:$I$15</xm:f>
           </x14:formula1>
@@ -33656,7 +33532,7 @@
           </x14:formula2>
           <xm:sqref>AF2:AH9 AU2:AU9 AW2:AZ6 BM2:BM9 BO2:BR6 DC2:DJ6 DZ2:EG4 ET2:EY44 DX5:DX6 EB5:EG6 AV6:AZ6 BN6:BR6 EA6:EG6 AV7:AV8 AX7:AZ9 BN7:BN8 BP7:BR9 DE7:DJ10 EC7:EG8 AW9:AZ10 BO9:BR10 EB9:EG9 AG10:AH10 AV10:AZ10 BN10:BR10 EC10:EG10 AY11:AZ14 BQ11:BR14 DC11:DJ13 EB11:EF13 DE14:DJ15 EB14:EB15 AW15:AZ15 BO15:BR15 AG16:AH16 AU16 AY16:AZ16 BM16 BQ16:BR16 DC16:DJ16 EA16:EG16 AZ17 BR17 DD17:DJ18 EA17:EB17 AW18:AZ19 BO18:BR19 EA18 AH19:AI19 DC19:DJ19 AH20:AH28 AX20:AZ23 BP20:BR23 DD20:DJ23 DC24:DJ28 DZ24:DZ28 AY29:AZ29 BQ29:BR29 DD29:DJ29 AG30:AH31 AV30:AZ31 BN30:BR31 DC30:DJ42 AH32:AH44 AX32:AZ38 BP32:BR38 AW39:AZ40 BO39:BR40 AV41:AZ44 BN41:BR44 DC45:DJ48 DC51:DJ59 DD60:DJ63 DC64:DJ73</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000048000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$P$2:$P$3</xm:f>
           </x14:formula1>
@@ -33665,7 +33541,7 @@
           </x14:formula2>
           <xm:sqref>Z2:Z73 AO2:AO73 BG2:BG73 BY2:BY73 CU2:CU73 CW2:CW5 DQ2:DQ73 DS2:DT6 EO2:ES73 CV6:CW6 CW7:CW15 DT7:DT8 DT10:DT14 DS11:DT14 CV16:CW16 DS16:DT31 CW17:CW23 CW29 CV30:CW36 DT32:DT44 DS33:DT36 CW37:CW44 DS38:DT38 CV39:CW39 DS40:DT44 AA43:AA44 CV45:CZ48 DU45:DW45 CD46 DS46:DW48 CW49:CW50 DS49:DT49 DV49:DW49 DU50:DW50 CV51:CZ51 DS51:DW54 CW52:CW53 CB54:CD54 CV54:CZ54 CW55 DS55:DT55 CV56:CZ58 DS56:DW56 DT57 CC58:CD58 DS58:DW59 CW59 CV60:CZ60 DT60:DT65 CW61 DS61:DT65 DV61:DW62 CV62:CZ62 CC63:CD63 CW63:CW65 CY63:CZ63 DU63:DW63 CD66:CD67 CW66:CZ71 DS66:DW69 CC68:CD71 DS70:DT70 DS71:DW73 CW72 CW73:CZ73</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000049000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Characteristics_overview!$B$9:$F$9</xm:f>
           </x14:formula1>
@@ -33674,7 +33550,7 @@
           </x14:formula2>
           <xm:sqref>O2:P7 P8:P73 O9:P51 O53:P54 O57:O59 O61:P73</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-00004A000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Characteristics_overview!$B$14:$M$14</xm:f>
           </x14:formula1>
@@ -33683,7 +33559,7 @@
           </x14:formula2>
           <xm:sqref>DK45:DK48 DX45:EH48 ET45:EY73 AV46:AZ46 BN46:BR46 CO46 AU47:AZ47 BO47:BR47 AV48:AZ48 BN48:BR48 DZ49:EG49 DX50:EH56 DK51 CO54 DK56:DK58 EA57:EG57 DX58:EH59 CO60 DK60 EA60:EG60 DY61:EG62 DK62 DX63:EH63 EA64:EG64 AU66:AZ73 BJ66:BO73 DK66:DK71 DX66:EH69 DX71:EH73 DK73</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-00004B000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Characteristics_overview!$B$15:$J$15</xm:f>
           </x14:formula1>
@@ -33692,7 +33568,7 @@
           </x14:formula2>
           <xm:sqref>AI2:AI18 AV2:AV5 BN2:BN5 AW7:AW8 BO7:BO8 AF10:AF44 AU10:AU15 BM10:BM15 AG11:AI15 AV11:AX14 BN11:BP14 DX11:EA14 EG11:EG13 ED14:EG14 AV15 BN15 EC15:EG15 AW16:AX16 BO16:BP16 DX16:DX18 DZ16:DZ18 AG17:AI18 AU17:AX17 BM17:BP17 DY17:DZ18 EC17:EG17 AU18:AV29 BM18:BN29 EB18:EG18 AG19:AG29 DA19:DB19 EA19:EG19 AI20:AI44 AW20:AW29 BO20:BO29 DZ20:EG20 EB21:EG22 AX24:AZ28 BP24:BR28 DX24:DY29 EA24:EG28 AH29:AI29 AX29 BP29 EC29:EG29 AU30:AU46 BM30:BM46 DY30:EG31 AG32:AG44 AV32:AW38 BN32:BO38 EB32:EG32 DX33:EG36 EB37:EG37 EA38:EG38 AV39:AV40 BN39:BN40 DX39:DY40 CE40:CF45 EC40:EG40 DX41:EG44 AV45:AZ45 BN45:BR45 BM47:BN47 AU48:AU52 BM48:BM50 AV49:AZ52 BN49:BR50 CE49:CF50 DX49:DY49 BM51:BR52 CE52 AV53 AX53:AZ53 BN53 BP53:BR53 AU54:AZ54 BM54:BR54 AW55:AZ57 BO55:BR57 AV56:AZ58 BN56:BR58 DX57:DY57 AU58:AZ65 BM58:BR65 DX60:DZ60 DX61:DX62 CE64 DA64 DX64:DZ64 DX70:EG70</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-00004C000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Characteristics_overview!$B$15:$K$15</xm:f>
           </x14:formula1>
@@ -33701,7 +33577,7 @@
           </x14:formula2>
           <xm:sqref>CE2:CN39 DX2:DY4 DA6:DB6 DZ6:DZ10 DX7:EB8 AV9 BN9 DX9:EA9 DX10:EB10 DA14:DD15 DX15:EA15 AV16 BN16 DA16:DB16 DY16 AY17 BQ17 DX19:DZ19 DA20:DC20 DX20:DY23 DB21:DC23 DZ21:EA22 DZ23:EG23 DA24:DB28 DA30:DB37 DX30:DX32 DY32:DZ32 DX37:EA37 DX38:DZ38 DA39:DB39 CG40:CN45 DB40:DB42 DZ40:EB40 DB43:DJ44 DA45:DB48 CE46:CN48 CG49:CN53 DC49:DJ50 CE51:CN51 DA51:DB51 CF52:CN52 AU53 AW53 BM53 BO53 CE53:CN63 AU55:AV55 BM55:BN55 AU56:AU57 BM56:BM57 DA56:DB58 DZ57 CF64:CN64 DB64 CE65:CN73 DX65:EG65 DA66:DB71 DB72 DA73:DB73</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-00004D000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Characteristics_overview!$B$9:$G$9</xm:f>
           </x14:formula1>
@@ -33710,7 +33586,7 @@
           </x14:formula2>
           <xm:sqref>O8 O52 O55:O56 O60</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-00004E000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$M$2:$M$49</xm:f>
           </x14:formula1>
@@ -33719,7 +33595,7 @@
           </x14:formula2>
           <xm:sqref>DL7:DL8 AK15 BB15 BT15 CP15 DL15 AJ20 AL20 BA20 BC20 BS20 BU20 AJ24:AJ28 AL24:AL28 BA24:BA28 BC24:BC28 BS24:BS28 BU24:BU28 CO24:CO28 CQ24:CQ28 EH24:EH28 EJ24:EJ28 AK38 BB38 BT38 CP38</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-00004F000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$L$2:$L$59</xm:f>
           </x14:formula1>
@@ -33728,7 +33604,7 @@
           </x14:formula2>
           <xm:sqref>AS16 BK16 DV16 AD20 AS20 BK20 CC20 CY20 DV20</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000050000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$M$2:$M$50</xm:f>
           </x14:formula1>
@@ -33737,7 +33613,7 @@
           </x14:formula2>
           <xm:sqref>AL38 BC38 BU38 CQ38 AK39 BB39 BT39 CP39 EI39 CO67</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000051000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$L$2:$L$60</xm:f>
           </x14:formula1>
@@ -33746,7 +33622,7 @@
           </x14:formula2>
           <xm:sqref>AC39 AR39 BJ39 DU39</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000052000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$L$2:$L$62</xm:f>
           </x14:formula1>
@@ -33755,7 +33631,7 @@
           </x14:formula2>
           <xm:sqref>AT51 BL51 CD51</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000053000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$L$2:$L$63</xm:f>
           </x14:formula1>
@@ -33764,7 +33640,7 @@
           </x14:formula2>
           <xm:sqref>AS53 BK53 CC53 CY53 AT55 BL55 CC55</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000054000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$L$2:$L$64</xm:f>
           </x14:formula1>
@@ -33773,7 +33649,7 @@
           </x14:formula2>
           <xm:sqref>AS61 BK61</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000055000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Characteristics_overview!$B$5:$AA$5</xm:f>
           </x14:formula1>
@@ -33782,7 +33658,7 @@
           </x14:formula2>
           <xm:sqref>R2:R33 R36:R73 Q72:R72</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000056000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'xlfile://root/users/karkaz/documents/workspace/c:/volumes/documents/evelina/  doctorate/c:/users/alber/documents/2015 lavori/wallingford/aggiornamenti di maggio 2016/[ladybird-data_2016-05-31 alberto gr 12-6.xlsx]charact_default'!#REF!</xm:f>
           </x14:formula1>
@@ -33791,7 +33667,7 @@
           </x14:formula2>
           <xm:sqref>DA2:DB5 DU5 DV6 DA7:DB13 DS15:DT15 DU16 DA17:DC18 DA21:DA23 DN21:DN22 EL21:EL22 CR22 CC29 CY29 DA29:DC29 DS37 DA38:DB38 CB39 DA40:DA44 CR43:CR44 DN43:DN44 EK43:EK44 DS45:DT45 DA49:DB50 DU49 DS50:DT50 DA52:DB55 CQ53 CR55 CB58 DA59:DB59 DA60:DC63 CQ61 DM61 EH61:EH62 DA65:DB65 DA72</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000057000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'xlfile://root/users/karkaz/documents/workspace/c:/volumes/documents/evelina/  doctorate/c:/users/alber/documents/2016 lavori/coccinelle/antonio soares/correzioni database 12.2016/[ladybird-data_2016-11-10 alberto.xlsx]charact_default'!#REF!</xm:f>
           </x14:formula1>
@@ -33800,7 +33676,7 @@
           </x14:formula2>
           <xm:sqref>CX2:CZ5 DY5:EA5 CY6:CZ13 DY6 CX7:CZ13 CY16:CZ18 CX17:CZ18 DK17:DK18 DM17:DM23 CX21:CY23 DZ29:EB29 DK38 DK49:DL50 DK52:DL55 DO54 DK59 DO60 DO62</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000058000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Characteristics_overview!$B$4:$AC$4</xm:f>
           </x14:formula1>
@@ -33809,7 +33685,7 @@
           </x14:formula2>
           <xm:sqref>I2:I73</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000059000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Characteristics_overview!$B$2:$Y$2</xm:f>
           </x14:formula1>
@@ -33818,7 +33694,7 @@
           </x14:formula2>
           <xm:sqref>N2:N73</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-00005A000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Characteristics_overview!$B$3:$H$3</xm:f>
           </x14:formula1>
@@ -33827,7 +33703,7 @@
           </x14:formula2>
           <xm:sqref>J2:M73</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-00005B000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Characteristics_overview!$B$5:$AC$5</xm:f>
           </x14:formula1>
@@ -33836,7 +33712,7 @@
           </x14:formula2>
           <xm:sqref>R34:R35</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-00005C000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$J$2:$J$45</xm:f>
           </x14:formula1>
@@ -33845,7 +33721,7 @@
           </x14:formula2>
           <xm:sqref>Q43:Q44</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-00005D000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$K$2:$K$5</xm:f>
           </x14:formula1>
@@ -33854,7 +33730,7 @@
           </x14:formula2>
           <xm:sqref>V2 V46:V48 V54 V59 V64 V68:V69</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-00005E000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$K$2:$K$6</xm:f>
           </x14:formula1>
@@ -33863,7 +33739,7 @@
           </x14:formula2>
           <xm:sqref>V45</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-00005F000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$K$2:$K$7</xm:f>
           </x14:formula1>
@@ -33872,7 +33748,7 @@
           </x14:formula2>
           <xm:sqref>V57</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000060000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$K$2:$K$8</xm:f>
           </x14:formula1>
@@ -33881,7 +33757,7 @@
           </x14:formula2>
           <xm:sqref>V58</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000061000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$K$2:$K$9</xm:f>
           </x14:formula1>
@@ -33890,7 +33766,7 @@
           </x14:formula2>
           <xm:sqref>V60:V61 V65 V72</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000062000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$K$2:$K$11</xm:f>
           </x14:formula1>
@@ -33899,7 +33775,7 @@
           </x14:formula2>
           <xm:sqref>V49:V50</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000063000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$K$2:$K$12</xm:f>
           </x14:formula1>
@@ -33908,7 +33784,7 @@
           </x14:formula2>
           <xm:sqref>V51 V71</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000064000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$K$2:$K$13</xm:f>
           </x14:formula1>
@@ -33917,7 +33793,7 @@
           </x14:formula2>
           <xm:sqref>V52</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000065000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$K$2:$K$14</xm:f>
           </x14:formula1>
@@ -33926,7 +33802,7 @@
           </x14:formula2>
           <xm:sqref>V53</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000066000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$K$2:$K$15</xm:f>
           </x14:formula1>
@@ -33935,7 +33811,7 @@
           </x14:formula2>
           <xm:sqref>V55</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000067000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$K$2:$K$16</xm:f>
           </x14:formula1>
@@ -33944,7 +33820,7 @@
           </x14:formula2>
           <xm:sqref>V56</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000068000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$K$2:$K$17</xm:f>
           </x14:formula1>
@@ -33953,7 +33829,7 @@
           </x14:formula2>
           <xm:sqref>V62</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000069000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$K$2:$K$18</xm:f>
           </x14:formula1>
@@ -33962,7 +33838,7 @@
           </x14:formula2>
           <xm:sqref>V63 V70</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-00006A000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$K$2:$K$10</xm:f>
           </x14:formula1>
@@ -33971,7 +33847,7 @@
           </x14:formula2>
           <xm:sqref>V3:V44 V66:V67</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-00006B000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$M$2:$M$51</xm:f>
           </x14:formula1>
@@ -33980,7 +33856,7 @@
           </x14:formula2>
           <xm:sqref>CO58</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-00006C000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$N$2:$N$27</xm:f>
           </x14:formula1>
@@ -33989,7 +33865,7 @@
           </x14:formula2>
           <xm:sqref>AM2 BD2 BV2 CR2:CR4 EK2:EN2 FB2 EK3:EL4 AM45 BD45:BD47 BV45:BV48 CR45 DN45:DO45 EK45:EN45 FB45 AM47:AM48 CR47:CR48 DN47:DO48 EK47:EN48 FB47:FB48 AM50:AM52 BD50:BD52 BV50:BV52 CR50:CR52 EK50:EN52 FB50:FB52 DN51:DO51 AM54 BD54 BV54 CR54 DN54 EK54:EN54 FB54 AM58:AM60 BD58:BD60 BV58:BV60 CR58:CR60 DN58:DO58 EK58:EN60 FB58:FB60 DN59:DN60 AM62:AM63 BD62:BD63 BV62:BV63 CR62:CR63 DN62:DN63 EM62:EN62 FB62:FB63 EK63:EN63 AM66:AM73 BD66:BD73 BT66:BV73 CR66:CR72 DN66:DO70 EK66:EN73 FB66:FB73 DN71:DN73</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-00006D000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$N$2:$N$28</xm:f>
           </x14:formula1>
@@ -33998,7 +33874,7 @@
           </x14:formula2>
           <xm:sqref>AM49 BD49 BV49 CR49 DN49:DN50 EK49:EN49 FB49 DN52 AM64 BD64 BV64 CR64 DN64 EK64:EN64 FB64</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-00006E000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$N$2:$N$31</xm:f>
           </x14:formula1>
@@ -34007,7 +33883,7 @@
           </x14:formula2>
           <xm:sqref>AM53 BD53 BV53 DN53 EK53:EN53 FB53</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-00006F000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$N$2:$N$33</xm:f>
           </x14:formula1>
@@ -34016,7 +33892,7 @@
           </x14:formula2>
           <xm:sqref>AM55:AM57 BD55:BD57 BV55:BV57 EK55:EN57 FB55:FB57 CR56:CR57 DN56 DN57:DO57</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000070000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$N$2:$N$34</xm:f>
           </x14:formula1>
@@ -34025,7 +33901,7 @@
           </x14:formula2>
           <xm:sqref>AM65 BD65 BV65 CR65 DN65 EK65 EM65:EN65 FB65</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000071000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$N$2:$N$35</xm:f>
           </x14:formula1>
@@ -34034,7 +33910,7 @@
           </x14:formula2>
           <xm:sqref>DN2:DN5 AM3:AM44 BD3:BD44 BV3:BV44 EM3:EN18 FB3:FB44 CR5:CR21 EK5:EN9 DN6:DO6 DN7:DN15 EH9 EL10:EN10 EK11:EN17 DN16:DO16 DN17:DN18 EK18:EK20 EL19:EN20 EM21:EN26 CR23:CR42 DN23:DN29 EL23:EN23 EK24:EN42 DN30:DO36 DN37:DN38 DN39:DO39 DN40:DN42 EL43:EN44 AM61 BD61 BV61 CR61 DN61 EM61:EN61 FB61 CR73</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000072000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$O$2:$O$25</xm:f>
           </x14:formula1>
@@ -34043,7 +33919,7 @@
           </x14:formula2>
           <xm:sqref>W47</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000073000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$K$2:$K$19</xm:f>
           </x14:formula1>
@@ -34052,7 +33928,7 @@
           </x14:formula2>
           <xm:sqref>V73</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000074000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$M$2:$M$52</xm:f>
           </x14:formula1>
@@ -34061,7 +33937,7 @@
           </x14:formula2>
           <xm:sqref>BS47 BA58 BS58 BA60 BS60</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000075000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Characteristics_overview!$B$6:$AT$6</xm:f>
           </x14:formula1>
@@ -34070,7 +33946,7 @@
           </x14:formula2>
           <xm:sqref>S2:S73</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000076000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Charact_default!$O$2:$O$26</xm:f>
           </x14:formula1>
@@ -34086,7 +33962,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U36"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
@@ -36295,13 +36171,13 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C1:P64"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="M23" sqref="M23"/>
+      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -37819,7 +37695,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BL19"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
@@ -39254,10 +39130,10 @@
         <v>1052</v>
       </c>
       <c r="I13" s="31" t="s">
-        <v>1101</v>
+        <v>1062</v>
       </c>
       <c r="J13" s="31" t="s">
-        <v>1100</v>
+        <v>1061</v>
       </c>
       <c r="K13" s="31" t="s">
         <v>1053</v>
@@ -39645,7 +39521,7 @@
       <c r="AX16" s="31" t="s">
         <v>148</v>
       </c>
-      <c r="AY16" s="177" t="s">
+      <c r="AY16" s="174" t="s">
         <v>843</v>
       </c>
       <c r="AZ16" s="1"/>
@@ -39905,3038 +39781,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:J73"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="1025" width="8.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A1" s="174" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="174" t="s">
-        <v>1061</v>
-      </c>
-      <c r="C1" s="174" t="s">
-        <v>1062</v>
-      </c>
-      <c r="D1" s="174" t="s">
-        <v>1063</v>
-      </c>
-      <c r="E1" s="174" t="s">
-        <v>1061</v>
-      </c>
-      <c r="F1" s="174" t="s">
-        <v>1062</v>
-      </c>
-      <c r="G1" s="174" t="s">
-        <v>1063</v>
-      </c>
-      <c r="H1" s="174" t="s">
-        <v>1061</v>
-      </c>
-      <c r="I1" s="174" t="s">
-        <v>1062</v>
-      </c>
-      <c r="J1" s="174" t="s">
-        <v>1063</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A2" s="174">
-        <v>1</v>
-      </c>
-      <c r="B2" s="174">
-        <v>1024</v>
-      </c>
-      <c r="C2" s="174">
-        <v>683</v>
-      </c>
-      <c r="D2" s="174" t="s">
-        <v>1064</v>
-      </c>
-      <c r="E2" s="174">
-        <v>1024</v>
-      </c>
-      <c r="F2" s="174">
-        <v>850</v>
-      </c>
-      <c r="G2" s="174" t="s">
-        <v>1065</v>
-      </c>
-      <c r="H2" s="174">
-        <v>1024</v>
-      </c>
-      <c r="I2" s="174">
-        <v>782</v>
-      </c>
-      <c r="J2" s="174" t="s">
-        <v>1066</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A3" s="174">
-        <v>2</v>
-      </c>
-      <c r="B3" s="174">
-        <v>1024</v>
-      </c>
-      <c r="C3" s="174">
-        <v>683</v>
-      </c>
-      <c r="D3" s="175" t="s">
-        <v>1067</v>
-      </c>
-      <c r="E3" s="174">
-        <v>1024</v>
-      </c>
-      <c r="F3" s="174">
-        <v>718</v>
-      </c>
-      <c r="G3" s="174" t="s">
-        <v>1066</v>
-      </c>
-      <c r="H3" s="174"/>
-      <c r="I3" s="174"/>
-      <c r="J3" s="174"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A4" s="174">
-        <v>3</v>
-      </c>
-      <c r="B4" s="174">
-        <v>1024</v>
-      </c>
-      <c r="C4" s="174">
-        <v>794</v>
-      </c>
-      <c r="D4" s="174" t="s">
-        <v>1068</v>
-      </c>
-      <c r="E4" s="174">
-        <v>1024</v>
-      </c>
-      <c r="F4" s="174">
-        <v>683</v>
-      </c>
-      <c r="G4" s="174" t="s">
-        <v>1064</v>
-      </c>
-      <c r="H4" s="174">
-        <v>1024</v>
-      </c>
-      <c r="I4" s="174">
-        <v>658</v>
-      </c>
-      <c r="J4" s="174" t="s">
-        <v>1066</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A5" s="174">
-        <v>4</v>
-      </c>
-      <c r="B5" s="174">
-        <v>1024</v>
-      </c>
-      <c r="C5" s="174">
-        <v>772</v>
-      </c>
-      <c r="D5" s="174" t="s">
-        <v>1069</v>
-      </c>
-      <c r="E5" s="174">
-        <v>1024</v>
-      </c>
-      <c r="F5" s="174">
-        <v>665</v>
-      </c>
-      <c r="G5" s="174" t="s">
-        <v>1069</v>
-      </c>
-      <c r="H5" s="174">
-        <v>1024</v>
-      </c>
-      <c r="I5" s="174">
-        <v>839</v>
-      </c>
-      <c r="J5" s="174" t="s">
-        <v>1070</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A6" s="174">
-        <v>5</v>
-      </c>
-      <c r="B6" s="174">
-        <v>1024</v>
-      </c>
-      <c r="C6" s="174">
-        <v>716</v>
-      </c>
-      <c r="D6" s="174" t="s">
-        <v>1071</v>
-      </c>
-      <c r="E6" s="174">
-        <v>1024</v>
-      </c>
-      <c r="F6" s="174">
-        <v>678</v>
-      </c>
-      <c r="G6" s="174" t="s">
-        <v>1066</v>
-      </c>
-      <c r="H6" s="174">
-        <v>1024</v>
-      </c>
-      <c r="I6" s="174">
-        <v>678</v>
-      </c>
-      <c r="J6" s="174" t="s">
-        <v>1066</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A7" s="174">
-        <v>6</v>
-      </c>
-      <c r="B7" s="174">
-        <v>1024</v>
-      </c>
-      <c r="C7" s="174">
-        <v>731</v>
-      </c>
-      <c r="D7" s="174" t="s">
-        <v>1072</v>
-      </c>
-      <c r="E7" s="174">
-        <v>1024</v>
-      </c>
-      <c r="F7" s="174">
-        <v>839</v>
-      </c>
-      <c r="G7" s="174" t="s">
-        <v>1073</v>
-      </c>
-      <c r="H7" s="174">
-        <v>1024</v>
-      </c>
-      <c r="I7" s="174">
-        <v>683</v>
-      </c>
-      <c r="J7" s="174" t="s">
-        <v>1069</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A8" s="174">
-        <v>7</v>
-      </c>
-      <c r="B8" s="174">
-        <v>1024</v>
-      </c>
-      <c r="C8" s="174">
-        <v>762</v>
-      </c>
-      <c r="D8" s="174" t="s">
-        <v>1066</v>
-      </c>
-      <c r="E8" s="174"/>
-      <c r="F8" s="174"/>
-      <c r="G8" s="174"/>
-      <c r="H8" s="174"/>
-      <c r="I8" s="174"/>
-      <c r="J8" s="174"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A9" s="174">
-        <v>8</v>
-      </c>
-      <c r="B9" s="174">
-        <v>1024</v>
-      </c>
-      <c r="C9" s="174">
-        <v>678</v>
-      </c>
-      <c r="D9" s="174" t="s">
-        <v>1066</v>
-      </c>
-      <c r="E9" s="174">
-        <v>1024</v>
-      </c>
-      <c r="F9" s="174">
-        <v>778</v>
-      </c>
-      <c r="G9" s="174" t="s">
-        <v>1066</v>
-      </c>
-      <c r="H9" s="174">
-        <v>1024</v>
-      </c>
-      <c r="I9" s="174">
-        <v>768</v>
-      </c>
-      <c r="J9" s="174" t="s">
-        <v>1074</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A10" s="174">
-        <v>9</v>
-      </c>
-      <c r="B10" s="174">
-        <v>1024</v>
-      </c>
-      <c r="C10" s="174">
-        <v>678</v>
-      </c>
-      <c r="D10" s="174" t="s">
-        <v>1066</v>
-      </c>
-      <c r="E10" s="174">
-        <v>1024</v>
-      </c>
-      <c r="F10" s="174">
-        <v>683</v>
-      </c>
-      <c r="G10" s="174" t="s">
-        <v>1064</v>
-      </c>
-      <c r="H10" s="174">
-        <v>1024</v>
-      </c>
-      <c r="I10" s="174">
-        <v>686</v>
-      </c>
-      <c r="J10" s="174" t="s">
-        <v>1066</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A11" s="174">
-        <v>10</v>
-      </c>
-      <c r="B11" s="174">
-        <v>1024</v>
-      </c>
-      <c r="C11" s="174">
-        <v>678</v>
-      </c>
-      <c r="D11" s="174" t="s">
-        <v>1066</v>
-      </c>
-      <c r="E11" s="174">
-        <v>1024</v>
-      </c>
-      <c r="F11" s="174">
-        <v>641</v>
-      </c>
-      <c r="G11" s="174" t="s">
-        <v>1069</v>
-      </c>
-      <c r="H11" s="174">
-        <v>1024</v>
-      </c>
-      <c r="I11" s="174">
-        <v>680</v>
-      </c>
-      <c r="J11" s="174" t="s">
-        <v>1073</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A12" s="174">
-        <v>11</v>
-      </c>
-      <c r="B12" s="174">
-        <v>1024</v>
-      </c>
-      <c r="C12" s="174">
-        <v>683</v>
-      </c>
-      <c r="D12" s="174" t="s">
-        <v>1064</v>
-      </c>
-      <c r="E12" s="174">
-        <v>1024</v>
-      </c>
-      <c r="F12" s="174">
-        <v>685</v>
-      </c>
-      <c r="G12" s="174" t="s">
-        <v>1073</v>
-      </c>
-      <c r="H12" s="174">
-        <v>1024</v>
-      </c>
-      <c r="I12" s="174">
-        <v>678</v>
-      </c>
-      <c r="J12" s="174" t="s">
-        <v>1066</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A13" s="174">
-        <v>12</v>
-      </c>
-      <c r="B13" s="174">
-        <v>1024</v>
-      </c>
-      <c r="C13" s="174">
-        <v>683</v>
-      </c>
-      <c r="D13" s="174" t="s">
-        <v>1075</v>
-      </c>
-      <c r="E13" s="174">
-        <v>1024</v>
-      </c>
-      <c r="F13" s="174">
-        <v>683</v>
-      </c>
-      <c r="G13" s="174" t="s">
-        <v>1075</v>
-      </c>
-      <c r="H13" s="174">
-        <v>1024</v>
-      </c>
-      <c r="I13" s="174">
-        <v>712</v>
-      </c>
-      <c r="J13" s="174" t="s">
-        <v>1064</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A14" s="174">
-        <v>13</v>
-      </c>
-      <c r="B14" s="174">
-        <v>1024</v>
-      </c>
-      <c r="C14" s="174">
-        <v>678</v>
-      </c>
-      <c r="D14" s="174" t="s">
-        <v>1073</v>
-      </c>
-      <c r="E14" s="174">
-        <v>1024</v>
-      </c>
-      <c r="F14" s="174">
-        <v>840</v>
-      </c>
-      <c r="G14" s="174" t="s">
-        <v>1073</v>
-      </c>
-      <c r="H14" s="174">
-        <v>1024</v>
-      </c>
-      <c r="I14" s="174">
-        <v>683</v>
-      </c>
-      <c r="J14" s="174" t="s">
-        <v>1076</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A15" s="174">
-        <v>14</v>
-      </c>
-      <c r="B15" s="174">
-        <v>1024</v>
-      </c>
-      <c r="C15" s="174">
-        <v>686</v>
-      </c>
-      <c r="D15" s="174" t="s">
-        <v>1066</v>
-      </c>
-      <c r="E15" s="174">
-        <v>1024</v>
-      </c>
-      <c r="F15" s="174">
-        <v>683</v>
-      </c>
-      <c r="G15" s="174" t="s">
-        <v>1064</v>
-      </c>
-      <c r="H15" s="174">
-        <v>1024</v>
-      </c>
-      <c r="I15" s="174">
-        <v>683</v>
-      </c>
-      <c r="J15" s="174" t="s">
-        <v>1064</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A16" s="174">
-        <v>15</v>
-      </c>
-      <c r="B16" s="174">
-        <v>1024</v>
-      </c>
-      <c r="C16" s="174">
-        <v>678</v>
-      </c>
-      <c r="D16" s="174" t="s">
-        <v>1066</v>
-      </c>
-      <c r="E16" s="174">
-        <v>1024</v>
-      </c>
-      <c r="F16" s="174">
-        <v>678</v>
-      </c>
-      <c r="G16" s="174" t="s">
-        <v>1066</v>
-      </c>
-      <c r="H16" s="174">
-        <v>1024</v>
-      </c>
-      <c r="I16" s="174">
-        <v>768</v>
-      </c>
-      <c r="J16" s="174" t="s">
-        <v>1077</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A17" s="174">
-        <v>16</v>
-      </c>
-      <c r="B17" s="174">
-        <v>1024</v>
-      </c>
-      <c r="C17" s="174">
-        <v>682</v>
-      </c>
-      <c r="D17" s="174" t="s">
-        <v>1075</v>
-      </c>
-      <c r="E17" s="174">
-        <v>1024</v>
-      </c>
-      <c r="F17" s="174">
-        <v>854</v>
-      </c>
-      <c r="G17" s="174" t="s">
-        <v>1064</v>
-      </c>
-      <c r="H17" s="174">
-        <v>1024</v>
-      </c>
-      <c r="I17" s="174">
-        <v>802</v>
-      </c>
-      <c r="J17" s="174" t="s">
-        <v>1078</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A18" s="174">
-        <v>17</v>
-      </c>
-      <c r="B18" s="174">
-        <v>1024</v>
-      </c>
-      <c r="C18" s="174">
-        <v>683</v>
-      </c>
-      <c r="D18" s="174" t="s">
-        <v>1064</v>
-      </c>
-      <c r="E18" s="174">
-        <v>1024</v>
-      </c>
-      <c r="F18" s="174">
-        <v>685</v>
-      </c>
-      <c r="G18" s="174" t="s">
-        <v>1066</v>
-      </c>
-      <c r="H18" s="174">
-        <v>1024</v>
-      </c>
-      <c r="I18" s="174">
-        <v>686</v>
-      </c>
-      <c r="J18" s="174" t="s">
-        <v>1066</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A19" s="174">
-        <v>18</v>
-      </c>
-      <c r="B19" s="174">
-        <v>1024</v>
-      </c>
-      <c r="C19" s="174">
-        <v>804</v>
-      </c>
-      <c r="D19" s="174" t="s">
-        <v>1073</v>
-      </c>
-      <c r="E19" s="174">
-        <v>1024</v>
-      </c>
-      <c r="F19" s="174">
-        <v>678</v>
-      </c>
-      <c r="G19" s="174" t="s">
-        <v>1066</v>
-      </c>
-      <c r="H19" s="174">
-        <v>1024</v>
-      </c>
-      <c r="I19" s="174">
-        <v>788</v>
-      </c>
-      <c r="J19" s="174" t="s">
-        <v>1073</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A20" s="174">
-        <v>19</v>
-      </c>
-      <c r="B20" s="174">
-        <v>1024</v>
-      </c>
-      <c r="C20" s="174">
-        <v>730</v>
-      </c>
-      <c r="D20" s="174" t="s">
-        <v>1072</v>
-      </c>
-      <c r="E20" s="174">
-        <v>1024</v>
-      </c>
-      <c r="F20" s="174">
-        <v>683</v>
-      </c>
-      <c r="G20" s="174" t="s">
-        <v>1079</v>
-      </c>
-      <c r="H20" s="174">
-        <v>1024</v>
-      </c>
-      <c r="I20" s="174">
-        <v>686</v>
-      </c>
-      <c r="J20" s="174" t="s">
-        <v>1066</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A21" s="174">
-        <v>20</v>
-      </c>
-      <c r="B21" s="174">
-        <v>1024</v>
-      </c>
-      <c r="C21" s="174">
-        <v>678</v>
-      </c>
-      <c r="D21" s="174" t="s">
-        <v>1066</v>
-      </c>
-      <c r="E21" s="174">
-        <v>1024</v>
-      </c>
-      <c r="F21" s="174">
-        <v>683</v>
-      </c>
-      <c r="G21" s="174" t="s">
-        <v>1064</v>
-      </c>
-      <c r="H21" s="174"/>
-      <c r="I21" s="174"/>
-      <c r="J21" s="174"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A22" s="174">
-        <v>21</v>
-      </c>
-      <c r="B22" s="174">
-        <v>1024</v>
-      </c>
-      <c r="C22" s="174">
-        <v>686</v>
-      </c>
-      <c r="D22" s="174" t="s">
-        <v>1066</v>
-      </c>
-      <c r="E22" s="174">
-        <v>1024</v>
-      </c>
-      <c r="F22" s="174">
-        <v>678</v>
-      </c>
-      <c r="G22" s="174" t="s">
-        <v>1066</v>
-      </c>
-      <c r="H22" s="174">
-        <v>1024</v>
-      </c>
-      <c r="I22" s="174">
-        <v>685</v>
-      </c>
-      <c r="J22" s="174" t="s">
-        <v>1066</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A23" s="174">
-        <v>22</v>
-      </c>
-      <c r="B23" s="174">
-        <v>1024</v>
-      </c>
-      <c r="C23" s="174">
-        <v>678</v>
-      </c>
-      <c r="D23" s="174" t="s">
-        <v>1066</v>
-      </c>
-      <c r="E23" s="174">
-        <v>1024</v>
-      </c>
-      <c r="F23" s="174">
-        <v>999</v>
-      </c>
-      <c r="G23" s="174" t="s">
-        <v>1080</v>
-      </c>
-      <c r="H23" s="174">
-        <v>1024</v>
-      </c>
-      <c r="I23" s="174">
-        <v>731</v>
-      </c>
-      <c r="J23" s="174" t="s">
-        <v>1080</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A24" s="174">
-        <v>23</v>
-      </c>
-      <c r="B24" s="174">
-        <v>1024</v>
-      </c>
-      <c r="C24" s="174">
-        <v>819</v>
-      </c>
-      <c r="D24" s="174" t="s">
-        <v>1081</v>
-      </c>
-      <c r="E24" s="174">
-        <v>1024</v>
-      </c>
-      <c r="F24" s="174">
-        <v>732</v>
-      </c>
-      <c r="G24" s="174" t="s">
-        <v>1072</v>
-      </c>
-      <c r="H24" s="174">
-        <v>1024</v>
-      </c>
-      <c r="I24" s="174">
-        <v>732</v>
-      </c>
-      <c r="J24" s="174" t="s">
-        <v>1072</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A25" s="174">
-        <v>24</v>
-      </c>
-      <c r="B25" s="174">
-        <v>1024</v>
-      </c>
-      <c r="C25" s="174">
-        <v>685</v>
-      </c>
-      <c r="D25" s="174" t="s">
-        <v>1082</v>
-      </c>
-      <c r="E25" s="174">
-        <v>1024</v>
-      </c>
-      <c r="F25" s="174">
-        <v>845</v>
-      </c>
-      <c r="G25" s="174" t="s">
-        <v>1073</v>
-      </c>
-      <c r="H25" s="174"/>
-      <c r="I25" s="174"/>
-      <c r="J25" s="174"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A26" s="174">
-        <v>25</v>
-      </c>
-      <c r="B26" s="174">
-        <v>1024</v>
-      </c>
-      <c r="C26" s="174">
-        <v>678</v>
-      </c>
-      <c r="D26" s="174" t="s">
-        <v>1066</v>
-      </c>
-      <c r="E26" s="174">
-        <v>1024</v>
-      </c>
-      <c r="F26" s="174">
-        <v>731</v>
-      </c>
-      <c r="G26" s="174" t="s">
-        <v>1072</v>
-      </c>
-      <c r="H26" s="174">
-        <v>1024</v>
-      </c>
-      <c r="I26" s="174">
-        <v>844</v>
-      </c>
-      <c r="J26" s="174" t="s">
-        <v>1064</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A27" s="174">
-        <v>26</v>
-      </c>
-      <c r="B27" s="174">
-        <v>1024</v>
-      </c>
-      <c r="C27" s="174">
-        <v>763</v>
-      </c>
-      <c r="D27" s="174" t="s">
-        <v>1071</v>
-      </c>
-      <c r="E27" s="174"/>
-      <c r="F27" s="174"/>
-      <c r="G27" s="174"/>
-      <c r="H27" s="174"/>
-      <c r="I27" s="174"/>
-      <c r="J27" s="174"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A28" s="174">
-        <v>27</v>
-      </c>
-      <c r="B28" s="174">
-        <v>1024</v>
-      </c>
-      <c r="C28" s="174">
-        <v>721</v>
-      </c>
-      <c r="D28" s="174" t="s">
-        <v>1083</v>
-      </c>
-      <c r="E28" s="174"/>
-      <c r="F28" s="174"/>
-      <c r="G28" s="174"/>
-      <c r="H28" s="174"/>
-      <c r="I28" s="174"/>
-      <c r="J28" s="174"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A29" s="174">
-        <v>28</v>
-      </c>
-      <c r="B29" s="174">
-        <v>1024</v>
-      </c>
-      <c r="C29" s="174">
-        <v>685</v>
-      </c>
-      <c r="D29" s="174" t="s">
-        <v>1066</v>
-      </c>
-      <c r="E29" s="174">
-        <v>1024</v>
-      </c>
-      <c r="F29" s="174">
-        <v>683</v>
-      </c>
-      <c r="G29" s="174" t="s">
-        <v>1064</v>
-      </c>
-      <c r="H29" s="174">
-        <v>1024</v>
-      </c>
-      <c r="I29" s="174">
-        <v>742</v>
-      </c>
-      <c r="J29" s="174" t="s">
-        <v>1073</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A30" s="174">
-        <v>29</v>
-      </c>
-      <c r="B30" s="174">
-        <v>1024</v>
-      </c>
-      <c r="C30" s="174">
-        <v>685</v>
-      </c>
-      <c r="D30" s="174" t="s">
-        <v>1066</v>
-      </c>
-      <c r="E30" s="174">
-        <v>1024</v>
-      </c>
-      <c r="F30" s="174">
-        <v>683</v>
-      </c>
-      <c r="G30" s="174" t="s">
-        <v>1064</v>
-      </c>
-      <c r="H30" s="174"/>
-      <c r="I30" s="174"/>
-      <c r="J30" s="174"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A31" s="174">
-        <v>30</v>
-      </c>
-      <c r="B31" s="174">
-        <v>1024</v>
-      </c>
-      <c r="C31" s="174">
-        <v>683</v>
-      </c>
-      <c r="D31" s="174" t="s">
-        <v>1064</v>
-      </c>
-      <c r="E31" s="174"/>
-      <c r="F31" s="174"/>
-      <c r="G31" s="174"/>
-      <c r="H31" s="174"/>
-      <c r="I31" s="174"/>
-      <c r="J31" s="174"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A32" s="174">
-        <v>31</v>
-      </c>
-      <c r="B32" s="174">
-        <v>1024</v>
-      </c>
-      <c r="C32" s="174">
-        <v>784</v>
-      </c>
-      <c r="D32" s="174" t="s">
-        <v>1084</v>
-      </c>
-      <c r="E32" s="174">
-        <v>1024</v>
-      </c>
-      <c r="F32" s="174">
-        <v>685</v>
-      </c>
-      <c r="G32" s="174" t="s">
-        <v>1066</v>
-      </c>
-      <c r="H32" s="174">
-        <v>1024</v>
-      </c>
-      <c r="I32" s="174">
-        <v>879</v>
-      </c>
-      <c r="J32" s="174" t="s">
-        <v>1064</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A33" s="174">
-        <v>32</v>
-      </c>
-      <c r="B33" s="174">
-        <v>1024</v>
-      </c>
-      <c r="C33" s="174">
-        <v>819</v>
-      </c>
-      <c r="D33" s="174" t="s">
-        <v>1085</v>
-      </c>
-      <c r="E33" s="174">
-        <v>1024</v>
-      </c>
-      <c r="F33" s="174">
-        <v>730</v>
-      </c>
-      <c r="G33" s="174" t="s">
-        <v>1072</v>
-      </c>
-      <c r="H33" s="174">
-        <v>1024</v>
-      </c>
-      <c r="I33" s="174">
-        <v>865</v>
-      </c>
-      <c r="J33" s="174" t="s">
-        <v>1064</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A34" s="174">
-        <v>33</v>
-      </c>
-      <c r="B34" s="174">
-        <v>1024</v>
-      </c>
-      <c r="C34" s="174">
-        <v>683</v>
-      </c>
-      <c r="D34" s="174" t="s">
-        <v>1086</v>
-      </c>
-      <c r="E34" s="174"/>
-      <c r="F34" s="174"/>
-      <c r="G34" s="174"/>
-      <c r="H34" s="174"/>
-      <c r="I34" s="174"/>
-      <c r="J34" s="174"/>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A35" s="174">
-        <v>34</v>
-      </c>
-      <c r="B35" s="174">
-        <v>1024</v>
-      </c>
-      <c r="C35" s="174">
-        <v>797</v>
-      </c>
-      <c r="D35" s="174" t="s">
-        <v>1087</v>
-      </c>
-      <c r="E35" s="174"/>
-      <c r="F35" s="174"/>
-      <c r="G35" s="174"/>
-      <c r="H35" s="174"/>
-      <c r="I35" s="174"/>
-      <c r="J35" s="174"/>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A36" s="174">
-        <v>35</v>
-      </c>
-      <c r="B36" s="174">
-        <v>1024</v>
-      </c>
-      <c r="C36" s="174">
-        <v>794</v>
-      </c>
-      <c r="D36" s="174" t="s">
-        <v>1087</v>
-      </c>
-      <c r="E36" s="174"/>
-      <c r="F36" s="174"/>
-      <c r="G36" s="174"/>
-      <c r="H36" s="174"/>
-      <c r="I36" s="174"/>
-      <c r="J36" s="174"/>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A37" s="174">
-        <v>36</v>
-      </c>
-      <c r="B37" s="174">
-        <v>1024</v>
-      </c>
-      <c r="C37" s="174">
-        <v>678</v>
-      </c>
-      <c r="D37" s="174" t="s">
-        <v>1066</v>
-      </c>
-      <c r="E37" s="174">
-        <v>1024</v>
-      </c>
-      <c r="F37" s="174">
-        <v>683</v>
-      </c>
-      <c r="G37" s="174" t="s">
-        <v>1088</v>
-      </c>
-      <c r="H37" s="174">
-        <v>1024</v>
-      </c>
-      <c r="I37" s="174">
-        <v>768</v>
-      </c>
-      <c r="J37" s="174" t="s">
-        <v>1089</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A38" s="174">
-        <v>37</v>
-      </c>
-      <c r="B38" s="174">
-        <v>1024</v>
-      </c>
-      <c r="C38" s="174">
-        <v>678</v>
-      </c>
-      <c r="D38" s="174" t="s">
-        <v>1066</v>
-      </c>
-      <c r="E38" s="174">
-        <v>1024</v>
-      </c>
-      <c r="F38" s="174">
-        <v>678</v>
-      </c>
-      <c r="G38" s="174" t="s">
-        <v>1066</v>
-      </c>
-      <c r="H38" s="174">
-        <v>1024</v>
-      </c>
-      <c r="I38" s="174">
-        <v>886</v>
-      </c>
-      <c r="J38" s="174" t="s">
-        <v>1073</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A39" s="174">
-        <v>38</v>
-      </c>
-      <c r="B39" s="174">
-        <v>1024</v>
-      </c>
-      <c r="C39" s="174">
-        <v>736</v>
-      </c>
-      <c r="D39" s="174" t="s">
-        <v>1084</v>
-      </c>
-      <c r="E39" s="174">
-        <v>1024</v>
-      </c>
-      <c r="F39" s="174">
-        <v>716</v>
-      </c>
-      <c r="G39" s="174" t="s">
-        <v>1064</v>
-      </c>
-      <c r="H39" s="174">
-        <v>1024</v>
-      </c>
-      <c r="I39" s="174">
-        <v>1357</v>
-      </c>
-      <c r="J39" s="174" t="s">
-        <v>1084</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A40" s="174">
-        <v>39</v>
-      </c>
-      <c r="B40" s="174">
-        <v>1024</v>
-      </c>
-      <c r="C40" s="174">
-        <v>683</v>
-      </c>
-      <c r="D40" s="174" t="s">
-        <v>1064</v>
-      </c>
-      <c r="E40" s="174">
-        <v>1024</v>
-      </c>
-      <c r="F40" s="174">
-        <v>781</v>
-      </c>
-      <c r="G40" s="174" t="s">
-        <v>1064</v>
-      </c>
-      <c r="H40" s="174">
-        <v>1024</v>
-      </c>
-      <c r="I40" s="174">
-        <v>686</v>
-      </c>
-      <c r="J40" s="174" t="s">
-        <v>1066</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A41" s="174">
-        <v>40</v>
-      </c>
-      <c r="B41" s="174">
-        <v>1024</v>
-      </c>
-      <c r="C41" s="174">
-        <v>875</v>
-      </c>
-      <c r="D41" s="174" t="s">
-        <v>1066</v>
-      </c>
-      <c r="E41" s="174">
-        <v>1024</v>
-      </c>
-      <c r="F41" s="174">
-        <v>678</v>
-      </c>
-      <c r="G41" s="174" t="s">
-        <v>1066</v>
-      </c>
-      <c r="H41" s="174">
-        <v>1024</v>
-      </c>
-      <c r="I41" s="174">
-        <v>682</v>
-      </c>
-      <c r="J41" s="174" t="s">
-        <v>1090</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A42" s="174">
-        <v>41</v>
-      </c>
-      <c r="B42" s="174">
-        <v>1024</v>
-      </c>
-      <c r="C42" s="174">
-        <v>685</v>
-      </c>
-      <c r="D42" s="174" t="s">
-        <v>1066</v>
-      </c>
-      <c r="E42" s="174">
-        <v>1024</v>
-      </c>
-      <c r="F42" s="174">
-        <v>828</v>
-      </c>
-      <c r="G42" s="174" t="s">
-        <v>1085</v>
-      </c>
-      <c r="H42" s="174">
-        <v>1024</v>
-      </c>
-      <c r="I42" s="174">
-        <v>685</v>
-      </c>
-      <c r="J42" s="174" t="s">
-        <v>1066</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A43" s="174">
-        <v>42</v>
-      </c>
-      <c r="B43" s="174">
-        <v>1024</v>
-      </c>
-      <c r="C43" s="174">
-        <v>1441</v>
-      </c>
-      <c r="D43" s="174" t="s">
-        <v>1091</v>
-      </c>
-      <c r="E43" s="174"/>
-      <c r="F43" s="174"/>
-      <c r="G43" s="174"/>
-      <c r="H43" s="174"/>
-      <c r="I43" s="174"/>
-      <c r="J43" s="174"/>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A44" s="174">
-        <v>43</v>
-      </c>
-      <c r="B44" s="174">
-        <v>1024</v>
-      </c>
-      <c r="C44" s="174">
-        <v>1364</v>
-      </c>
-      <c r="D44" s="174" t="s">
-        <v>1091</v>
-      </c>
-      <c r="E44" s="174"/>
-      <c r="F44" s="174"/>
-      <c r="G44" s="174"/>
-      <c r="H44" s="174"/>
-      <c r="I44" s="174"/>
-      <c r="J44" s="174"/>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A45" s="174">
-        <v>44</v>
-      </c>
-      <c r="B45" s="174">
-        <v>1024</v>
-      </c>
-      <c r="C45" s="174">
-        <v>678</v>
-      </c>
-      <c r="D45" s="174" t="s">
-        <v>1066</v>
-      </c>
-      <c r="E45" s="174">
-        <v>1024</v>
-      </c>
-      <c r="F45" s="174">
-        <v>678</v>
-      </c>
-      <c r="G45" s="174" t="s">
-        <v>1066</v>
-      </c>
-      <c r="H45" s="174"/>
-      <c r="I45" s="174"/>
-      <c r="J45" s="174"/>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A46" s="174">
-        <v>45</v>
-      </c>
-      <c r="B46" s="174">
-        <v>1024</v>
-      </c>
-      <c r="C46" s="174">
-        <v>1343</v>
-      </c>
-      <c r="D46" s="174" t="s">
-        <v>1092</v>
-      </c>
-      <c r="E46" s="174"/>
-      <c r="F46" s="174"/>
-      <c r="G46" s="174"/>
-      <c r="H46" s="174"/>
-      <c r="I46" s="174"/>
-      <c r="J46" s="174"/>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A47" s="174">
-        <v>46</v>
-      </c>
-      <c r="B47" s="174">
-        <v>1024</v>
-      </c>
-      <c r="C47" s="174">
-        <v>780</v>
-      </c>
-      <c r="D47" s="174" t="s">
-        <v>1092</v>
-      </c>
-      <c r="E47" s="174"/>
-      <c r="F47" s="174"/>
-      <c r="G47" s="174"/>
-      <c r="H47" s="174"/>
-      <c r="I47" s="174"/>
-      <c r="J47" s="174"/>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A48" s="174">
-        <v>47</v>
-      </c>
-      <c r="B48" s="174">
-        <v>1024</v>
-      </c>
-      <c r="C48" s="174">
-        <v>881</v>
-      </c>
-      <c r="D48" s="174" t="s">
-        <v>1092</v>
-      </c>
-      <c r="E48" s="174"/>
-      <c r="F48" s="174"/>
-      <c r="G48" s="174"/>
-      <c r="H48" s="174"/>
-      <c r="I48" s="174"/>
-      <c r="J48" s="174"/>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A49" s="174">
-        <v>48</v>
-      </c>
-      <c r="B49" s="174">
-        <v>1024</v>
-      </c>
-      <c r="C49" s="174">
-        <v>685</v>
-      </c>
-      <c r="D49" s="174" t="s">
-        <v>1066</v>
-      </c>
-      <c r="E49" s="174">
-        <v>1024</v>
-      </c>
-      <c r="F49" s="174">
-        <v>686</v>
-      </c>
-      <c r="G49" s="174" t="s">
-        <v>1066</v>
-      </c>
-      <c r="H49" s="174">
-        <v>1024</v>
-      </c>
-      <c r="I49" s="174">
-        <v>678</v>
-      </c>
-      <c r="J49" s="174" t="s">
-        <v>1066</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A50" s="174">
-        <v>49</v>
-      </c>
-      <c r="B50" s="174">
-        <v>1024</v>
-      </c>
-      <c r="C50" s="174">
-        <v>678</v>
-      </c>
-      <c r="D50" s="174" t="s">
-        <v>1066</v>
-      </c>
-      <c r="E50" s="174">
-        <v>1024</v>
-      </c>
-      <c r="F50" s="174">
-        <v>1365</v>
-      </c>
-      <c r="G50" s="174" t="s">
-        <v>1092</v>
-      </c>
-      <c r="H50" s="174"/>
-      <c r="I50" s="174"/>
-      <c r="J50" s="174"/>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A51" s="174">
-        <v>50</v>
-      </c>
-      <c r="B51" s="174">
-        <v>1024</v>
-      </c>
-      <c r="C51" s="174">
-        <v>685</v>
-      </c>
-      <c r="D51" s="174" t="s">
-        <v>1066</v>
-      </c>
-      <c r="E51" s="174">
-        <v>1024</v>
-      </c>
-      <c r="F51" s="174">
-        <v>686</v>
-      </c>
-      <c r="G51" s="174" t="s">
-        <v>1066</v>
-      </c>
-      <c r="H51" s="174">
-        <v>1024</v>
-      </c>
-      <c r="I51" s="174">
-        <v>1365</v>
-      </c>
-      <c r="J51" s="174" t="s">
-        <v>1092</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A52" s="174">
-        <v>51</v>
-      </c>
-      <c r="B52" s="174">
-        <v>1024</v>
-      </c>
-      <c r="C52" s="174">
-        <v>685</v>
-      </c>
-      <c r="D52" s="174" t="s">
-        <v>1066</v>
-      </c>
-      <c r="E52" s="174">
-        <v>1024</v>
-      </c>
-      <c r="F52" s="174">
-        <v>769</v>
-      </c>
-      <c r="G52" s="174" t="s">
-        <v>1093</v>
-      </c>
-      <c r="H52" s="174">
-        <v>1024</v>
-      </c>
-      <c r="I52" s="174">
-        <v>1365</v>
-      </c>
-      <c r="J52" s="174" t="s">
-        <v>1092</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A53" s="174">
-        <v>52</v>
-      </c>
-      <c r="B53" s="174">
-        <v>1024</v>
-      </c>
-      <c r="C53" s="174">
-        <v>686</v>
-      </c>
-      <c r="D53" s="174" t="s">
-        <v>1066</v>
-      </c>
-      <c r="E53" s="174">
-        <v>1024</v>
-      </c>
-      <c r="F53" s="174">
-        <v>686</v>
-      </c>
-      <c r="G53" s="174" t="s">
-        <v>1066</v>
-      </c>
-      <c r="H53" s="174">
-        <v>1024</v>
-      </c>
-      <c r="I53" s="174">
-        <v>686</v>
-      </c>
-      <c r="J53" s="174" t="s">
-        <v>1066</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A54" s="174">
-        <v>53</v>
-      </c>
-      <c r="B54" s="174">
-        <v>1024</v>
-      </c>
-      <c r="C54" s="174">
-        <v>796</v>
-      </c>
-      <c r="D54" s="174" t="s">
-        <v>1094</v>
-      </c>
-      <c r="E54" s="174"/>
-      <c r="F54" s="174"/>
-      <c r="G54" s="174"/>
-      <c r="H54" s="174"/>
-      <c r="I54" s="174"/>
-      <c r="J54" s="174"/>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A55" s="174">
-        <v>54</v>
-      </c>
-      <c r="B55" s="174">
-        <v>1024</v>
-      </c>
-      <c r="C55" s="174">
-        <v>686</v>
-      </c>
-      <c r="D55" s="174" t="s">
-        <v>1066</v>
-      </c>
-      <c r="E55" s="174">
-        <v>1024</v>
-      </c>
-      <c r="F55" s="174">
-        <v>686</v>
-      </c>
-      <c r="G55" s="174" t="s">
-        <v>1066</v>
-      </c>
-      <c r="H55" s="174">
-        <v>1024</v>
-      </c>
-      <c r="I55" s="174">
-        <v>1365</v>
-      </c>
-      <c r="J55" s="174" t="s">
-        <v>1092</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A56" s="174">
-        <v>55</v>
-      </c>
-      <c r="B56" s="174">
-        <v>1024</v>
-      </c>
-      <c r="C56" s="174">
-        <v>686</v>
-      </c>
-      <c r="D56" s="174" t="s">
-        <v>1066</v>
-      </c>
-      <c r="E56" s="174">
-        <v>1024</v>
-      </c>
-      <c r="F56" s="174">
-        <v>1148</v>
-      </c>
-      <c r="G56" s="174" t="s">
-        <v>1094</v>
-      </c>
-      <c r="H56" s="174"/>
-      <c r="I56" s="174"/>
-      <c r="J56" s="174"/>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A57" s="174">
-        <v>56</v>
-      </c>
-      <c r="B57" s="174">
-        <v>1024</v>
-      </c>
-      <c r="C57" s="174">
-        <v>678</v>
-      </c>
-      <c r="D57" s="174" t="s">
-        <v>1066</v>
-      </c>
-      <c r="E57" s="174">
-        <v>1024</v>
-      </c>
-      <c r="F57" s="174">
-        <v>678</v>
-      </c>
-      <c r="G57" s="174" t="s">
-        <v>1066</v>
-      </c>
-      <c r="H57" s="174">
-        <v>1024</v>
-      </c>
-      <c r="I57" s="174">
-        <v>678</v>
-      </c>
-      <c r="J57" s="174" t="s">
-        <v>1066</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A58" s="174">
-        <v>57</v>
-      </c>
-      <c r="B58" s="174">
-        <v>1024</v>
-      </c>
-      <c r="C58" s="174">
-        <v>1365</v>
-      </c>
-      <c r="D58" s="174" t="s">
-        <v>1092</v>
-      </c>
-      <c r="E58" s="174"/>
-      <c r="F58" s="174"/>
-      <c r="G58" s="174"/>
-      <c r="H58" s="174"/>
-      <c r="I58" s="174"/>
-      <c r="J58" s="174"/>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A59" s="174">
-        <v>58</v>
-      </c>
-      <c r="B59" s="174">
-        <v>1024</v>
-      </c>
-      <c r="C59" s="174">
-        <v>1212</v>
-      </c>
-      <c r="D59" s="174" t="s">
-        <v>1092</v>
-      </c>
-      <c r="E59" s="174"/>
-      <c r="F59" s="174"/>
-      <c r="G59" s="174"/>
-      <c r="H59" s="174"/>
-      <c r="I59" s="174"/>
-      <c r="J59" s="174"/>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A60" s="174">
-        <v>59</v>
-      </c>
-      <c r="B60" s="174">
-        <v>1024</v>
-      </c>
-      <c r="C60" s="174">
-        <v>678</v>
-      </c>
-      <c r="D60" s="174" t="s">
-        <v>1066</v>
-      </c>
-      <c r="E60" s="174">
-        <v>1024</v>
-      </c>
-      <c r="F60" s="174">
-        <v>678</v>
-      </c>
-      <c r="G60" s="174" t="s">
-        <v>1066</v>
-      </c>
-      <c r="H60" s="174">
-        <v>1024</v>
-      </c>
-      <c r="I60" s="174">
-        <v>678</v>
-      </c>
-      <c r="J60" s="174" t="s">
-        <v>1066</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A61" s="174">
-        <v>60</v>
-      </c>
-      <c r="B61" s="174">
-        <v>1024</v>
-      </c>
-      <c r="C61" s="174">
-        <v>686</v>
-      </c>
-      <c r="D61" s="174" t="s">
-        <v>1066</v>
-      </c>
-      <c r="E61" s="174">
-        <v>1024</v>
-      </c>
-      <c r="F61" s="174">
-        <v>686</v>
-      </c>
-      <c r="G61" s="174" t="s">
-        <v>1066</v>
-      </c>
-      <c r="H61" s="174">
-        <v>1024</v>
-      </c>
-      <c r="I61" s="174">
-        <v>685</v>
-      </c>
-      <c r="J61" s="174" t="s">
-        <v>1066</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A62" s="174">
-        <v>61</v>
-      </c>
-      <c r="B62" s="174">
-        <v>1024</v>
-      </c>
-      <c r="C62" s="174">
-        <v>683</v>
-      </c>
-      <c r="D62" s="174" t="s">
-        <v>1066</v>
-      </c>
-      <c r="E62" s="174">
-        <v>1024</v>
-      </c>
-      <c r="F62" s="174">
-        <v>1365</v>
-      </c>
-      <c r="G62" s="174" t="s">
-        <v>1092</v>
-      </c>
-      <c r="H62" s="174"/>
-      <c r="I62" s="174"/>
-      <c r="J62" s="174"/>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A63" s="174">
-        <v>62</v>
-      </c>
-      <c r="B63" s="174">
-        <v>1024</v>
-      </c>
-      <c r="C63" s="174">
-        <v>686</v>
-      </c>
-      <c r="D63" s="174" t="s">
-        <v>1066</v>
-      </c>
-      <c r="E63" s="174">
-        <v>1024</v>
-      </c>
-      <c r="F63" s="174">
-        <v>1145</v>
-      </c>
-      <c r="G63" s="174" t="s">
-        <v>1094</v>
-      </c>
-      <c r="H63" s="174"/>
-      <c r="I63" s="174"/>
-      <c r="J63" s="174"/>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A64" s="174">
-        <v>63</v>
-      </c>
-      <c r="B64" s="174">
-        <v>1024</v>
-      </c>
-      <c r="C64" s="174">
-        <v>740</v>
-      </c>
-      <c r="D64" s="174" t="s">
-        <v>1066</v>
-      </c>
-      <c r="E64" s="174">
-        <v>1024</v>
-      </c>
-      <c r="F64" s="174">
-        <v>772</v>
-      </c>
-      <c r="G64" s="174" t="s">
-        <v>1066</v>
-      </c>
-      <c r="H64" s="174"/>
-      <c r="I64" s="174"/>
-      <c r="J64" s="174"/>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A65" s="174">
-        <v>64</v>
-      </c>
-      <c r="B65" s="174">
-        <v>1024</v>
-      </c>
-      <c r="C65" s="174">
-        <v>678</v>
-      </c>
-      <c r="D65" s="174" t="s">
-        <v>1066</v>
-      </c>
-      <c r="E65" s="174">
-        <v>1024</v>
-      </c>
-      <c r="F65" s="174">
-        <v>787</v>
-      </c>
-      <c r="G65" s="174" t="s">
-        <v>1066</v>
-      </c>
-      <c r="H65" s="174">
-        <v>1024</v>
-      </c>
-      <c r="I65" s="174">
-        <v>678</v>
-      </c>
-      <c r="J65" s="174" t="s">
-        <v>1066</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A66" s="174">
-        <v>65</v>
-      </c>
-      <c r="B66" s="174">
-        <v>1024</v>
-      </c>
-      <c r="C66" s="174">
-        <v>795</v>
-      </c>
-      <c r="D66" s="174" t="s">
-        <v>1094</v>
-      </c>
-      <c r="E66" s="174"/>
-      <c r="F66" s="174"/>
-      <c r="G66" s="174"/>
-      <c r="H66" s="174"/>
-      <c r="I66" s="174"/>
-      <c r="J66" s="174"/>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A67" s="174">
-        <v>66</v>
-      </c>
-      <c r="B67" s="174">
-        <v>1024</v>
-      </c>
-      <c r="C67" s="174">
-        <v>747</v>
-      </c>
-      <c r="D67" s="174" t="s">
-        <v>1094</v>
-      </c>
-      <c r="E67" s="174"/>
-      <c r="F67" s="174"/>
-      <c r="G67" s="174"/>
-      <c r="H67" s="174"/>
-      <c r="I67" s="174"/>
-      <c r="J67" s="174"/>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A68" s="174">
-        <v>67</v>
-      </c>
-      <c r="B68" s="174">
-        <v>1024</v>
-      </c>
-      <c r="C68" s="174">
-        <v>707</v>
-      </c>
-      <c r="D68" s="174" t="s">
-        <v>1095</v>
-      </c>
-      <c r="E68" s="174">
-        <v>1024</v>
-      </c>
-      <c r="F68" s="174">
-        <v>683</v>
-      </c>
-      <c r="G68" s="174" t="s">
-        <v>1096</v>
-      </c>
-      <c r="H68" s="174"/>
-      <c r="I68" s="174"/>
-      <c r="J68" s="174"/>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A69" s="174">
-        <v>68</v>
-      </c>
-      <c r="B69" s="174">
-        <v>1024</v>
-      </c>
-      <c r="C69" s="174">
-        <v>821</v>
-      </c>
-      <c r="D69" s="174" t="s">
-        <v>1097</v>
-      </c>
-      <c r="E69" s="174">
-        <v>1024</v>
-      </c>
-      <c r="F69" s="174">
-        <v>1001</v>
-      </c>
-      <c r="G69" s="174" t="s">
-        <v>1097</v>
-      </c>
-      <c r="H69" s="174">
-        <v>1024</v>
-      </c>
-      <c r="I69" s="174">
-        <v>823</v>
-      </c>
-      <c r="J69" s="174" t="s">
-        <v>1097</v>
-      </c>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A70" s="174">
-        <v>69</v>
-      </c>
-      <c r="B70" s="174">
-        <v>1024</v>
-      </c>
-      <c r="C70" s="174">
-        <v>1365</v>
-      </c>
-      <c r="D70" s="174" t="s">
-        <v>1092</v>
-      </c>
-      <c r="E70" s="174"/>
-      <c r="F70" s="174"/>
-      <c r="G70" s="174"/>
-      <c r="H70" s="174"/>
-      <c r="I70" s="174"/>
-      <c r="J70" s="174"/>
-    </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A71" s="174">
-        <v>70</v>
-      </c>
-      <c r="B71" s="174">
-        <v>1024</v>
-      </c>
-      <c r="C71" s="174">
-        <v>776</v>
-      </c>
-      <c r="D71" s="174" t="s">
-        <v>1094</v>
-      </c>
-      <c r="E71" s="174"/>
-      <c r="F71" s="174"/>
-      <c r="G71" s="174"/>
-      <c r="H71" s="174"/>
-      <c r="I71" s="174"/>
-      <c r="J71" s="174"/>
-    </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A72" s="174">
-        <v>71</v>
-      </c>
-      <c r="B72" s="174">
-        <v>1024</v>
-      </c>
-      <c r="C72" s="174">
-        <v>678</v>
-      </c>
-      <c r="D72" s="174" t="s">
-        <v>1066</v>
-      </c>
-      <c r="E72" s="174">
-        <v>1024</v>
-      </c>
-      <c r="F72" s="174">
-        <v>678</v>
-      </c>
-      <c r="G72" s="174" t="s">
-        <v>1066</v>
-      </c>
-      <c r="H72" s="174">
-        <v>1024</v>
-      </c>
-      <c r="I72" s="174">
-        <v>678</v>
-      </c>
-      <c r="J72" s="174" t="s">
-        <v>1066</v>
-      </c>
-    </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A73" s="174">
-        <v>72</v>
-      </c>
-      <c r="B73" s="174">
-        <v>1024</v>
-      </c>
-      <c r="C73" s="174">
-        <v>839</v>
-      </c>
-      <c r="D73" s="174" t="s">
-        <v>1098</v>
-      </c>
-      <c r="E73" s="174"/>
-      <c r="F73" s="174"/>
-      <c r="G73" s="174"/>
-      <c r="H73" s="174"/>
-      <c r="I73" s="174"/>
-      <c r="J73" s="174"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:M32"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="1" width="8.83203125" customWidth="1"/>
-    <col min="2" max="2" width="34.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17.33203125" style="5" customWidth="1"/>
-    <col min="5" max="1025" width="8.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A1" s="174" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="174"/>
-      <c r="C1" s="174"/>
-      <c r="D1" s="176" t="s">
-        <v>1099</v>
-      </c>
-      <c r="E1" s="174" t="s">
-        <v>1061</v>
-      </c>
-      <c r="F1" s="174" t="s">
-        <v>1062</v>
-      </c>
-      <c r="G1" s="174" t="s">
-        <v>1063</v>
-      </c>
-      <c r="H1" s="174" t="s">
-        <v>1061</v>
-      </c>
-      <c r="I1" s="174" t="s">
-        <v>1062</v>
-      </c>
-      <c r="J1" s="174" t="s">
-        <v>1063</v>
-      </c>
-      <c r="K1" s="174" t="s">
-        <v>1061</v>
-      </c>
-      <c r="L1" s="174" t="s">
-        <v>1062</v>
-      </c>
-      <c r="M1" s="174" t="s">
-        <v>1063</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="174">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C2" s="25" t="s">
-        <v>102</v>
-      </c>
-      <c r="D2" s="122">
-        <v>2</v>
-      </c>
-      <c r="E2" s="174">
-        <v>1024</v>
-      </c>
-      <c r="F2" s="174">
-        <v>683</v>
-      </c>
-      <c r="G2" s="174" t="s">
-        <v>1067</v>
-      </c>
-      <c r="H2" s="174">
-        <v>1024</v>
-      </c>
-      <c r="I2" s="174">
-        <v>718</v>
-      </c>
-      <c r="J2" s="174" t="s">
-        <v>1066</v>
-      </c>
-      <c r="K2" s="174"/>
-      <c r="L2" s="174"/>
-      <c r="M2" s="174"/>
-    </row>
-    <row r="3" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="174">
-        <v>7</v>
-      </c>
-      <c r="B3" s="25" t="s">
-        <v>156</v>
-      </c>
-      <c r="C3" s="48" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="176">
-        <v>2</v>
-      </c>
-      <c r="E3" s="174">
-        <v>1024</v>
-      </c>
-      <c r="F3" s="174">
-        <v>762</v>
-      </c>
-      <c r="G3" s="174" t="s">
-        <v>1066</v>
-      </c>
-      <c r="H3" s="174"/>
-      <c r="I3" s="174"/>
-      <c r="J3" s="174"/>
-      <c r="K3" s="174"/>
-      <c r="L3" s="174"/>
-      <c r="M3" s="174"/>
-    </row>
-    <row r="4" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="174">
-        <v>20</v>
-      </c>
-      <c r="B4" s="31" t="s">
-        <v>356</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>357</v>
-      </c>
-      <c r="D4" s="176">
-        <v>1</v>
-      </c>
-      <c r="E4" s="174">
-        <v>1024</v>
-      </c>
-      <c r="F4" s="174">
-        <v>678</v>
-      </c>
-      <c r="G4" s="174" t="s">
-        <v>1066</v>
-      </c>
-      <c r="H4" s="174">
-        <v>1024</v>
-      </c>
-      <c r="I4" s="174">
-        <v>683</v>
-      </c>
-      <c r="J4" s="174" t="s">
-        <v>1064</v>
-      </c>
-      <c r="K4" s="174"/>
-      <c r="L4" s="174"/>
-      <c r="M4" s="174"/>
-    </row>
-    <row r="5" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="174">
-        <v>24</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>395</v>
-      </c>
-      <c r="C5" s="24" t="s">
-        <v>412</v>
-      </c>
-      <c r="D5" s="176">
-        <v>1</v>
-      </c>
-      <c r="E5" s="174">
-        <v>1024</v>
-      </c>
-      <c r="F5" s="174">
-        <v>685</v>
-      </c>
-      <c r="G5" s="174" t="s">
-        <v>1082</v>
-      </c>
-      <c r="H5" s="174">
-        <v>1024</v>
-      </c>
-      <c r="I5" s="174">
-        <v>845</v>
-      </c>
-      <c r="J5" s="174" t="s">
-        <v>1073</v>
-      </c>
-      <c r="K5" s="174"/>
-      <c r="L5" s="174"/>
-      <c r="M5" s="174"/>
-    </row>
-    <row r="6" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="174">
-        <v>26</v>
-      </c>
-      <c r="B6" s="24" t="s">
-        <v>395</v>
-      </c>
-      <c r="C6" s="24" t="s">
-        <v>417</v>
-      </c>
-      <c r="D6" s="176">
-        <v>2</v>
-      </c>
-      <c r="E6" s="174">
-        <v>1024</v>
-      </c>
-      <c r="F6" s="174">
-        <v>763</v>
-      </c>
-      <c r="G6" s="174" t="s">
-        <v>1071</v>
-      </c>
-      <c r="H6" s="174"/>
-      <c r="I6" s="174"/>
-      <c r="J6" s="174"/>
-      <c r="K6" s="174"/>
-      <c r="L6" s="174"/>
-      <c r="M6" s="174"/>
-    </row>
-    <row r="7" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="174">
-        <v>27</v>
-      </c>
-      <c r="B7" s="24" t="s">
-        <v>395</v>
-      </c>
-      <c r="C7" s="24" t="s">
-        <v>418</v>
-      </c>
-      <c r="D7" s="176">
-        <v>2</v>
-      </c>
-      <c r="E7" s="174">
-        <v>1024</v>
-      </c>
-      <c r="F7" s="174">
-        <v>721</v>
-      </c>
-      <c r="G7" s="174" t="s">
-        <v>1083</v>
-      </c>
-      <c r="H7" s="174"/>
-      <c r="I7" s="174"/>
-      <c r="J7" s="174"/>
-      <c r="K7" s="174"/>
-      <c r="L7" s="174"/>
-      <c r="M7" s="174"/>
-    </row>
-    <row r="8" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="174">
-        <v>29</v>
-      </c>
-      <c r="B8" s="25" t="s">
-        <v>436</v>
-      </c>
-      <c r="C8" s="24" t="s">
-        <v>228</v>
-      </c>
-      <c r="D8" s="176">
-        <v>1</v>
-      </c>
-      <c r="E8" s="174">
-        <v>1024</v>
-      </c>
-      <c r="F8" s="174">
-        <v>685</v>
-      </c>
-      <c r="G8" s="174" t="s">
-        <v>1066</v>
-      </c>
-      <c r="H8" s="174">
-        <v>1024</v>
-      </c>
-      <c r="I8" s="174">
-        <v>683</v>
-      </c>
-      <c r="J8" s="174" t="s">
-        <v>1064</v>
-      </c>
-      <c r="K8" s="174"/>
-      <c r="L8" s="174"/>
-      <c r="M8" s="174"/>
-    </row>
-    <row r="9" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="174">
-        <v>30</v>
-      </c>
-      <c r="B9" s="24" t="s">
-        <v>436</v>
-      </c>
-      <c r="C9" s="24" t="s">
-        <v>449</v>
-      </c>
-      <c r="D9" s="176">
-        <v>2</v>
-      </c>
-      <c r="E9" s="174">
-        <v>1024</v>
-      </c>
-      <c r="F9" s="174">
-        <v>683</v>
-      </c>
-      <c r="G9" s="174" t="s">
-        <v>1064</v>
-      </c>
-      <c r="H9" s="174"/>
-      <c r="I9" s="174"/>
-      <c r="J9" s="174"/>
-      <c r="K9" s="174"/>
-      <c r="L9" s="174"/>
-      <c r="M9" s="174"/>
-    </row>
-    <row r="10" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="174">
-        <v>33</v>
-      </c>
-      <c r="B10" s="25" t="s">
-        <v>462</v>
-      </c>
-      <c r="C10" s="24" t="s">
-        <v>478</v>
-      </c>
-      <c r="D10" s="176">
-        <v>2</v>
-      </c>
-      <c r="E10" s="174">
-        <v>1024</v>
-      </c>
-      <c r="F10" s="174">
-        <v>683</v>
-      </c>
-      <c r="G10" s="174" t="s">
-        <v>1086</v>
-      </c>
-      <c r="H10" s="174"/>
-      <c r="I10" s="174"/>
-      <c r="J10" s="174"/>
-      <c r="K10" s="174"/>
-      <c r="L10" s="174"/>
-      <c r="M10" s="174"/>
-    </row>
-    <row r="11" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="174">
-        <v>34</v>
-      </c>
-      <c r="B11" s="24" t="s">
-        <v>462</v>
-      </c>
-      <c r="C11" s="24" t="s">
-        <v>480</v>
-      </c>
-      <c r="D11" s="176">
-        <v>2</v>
-      </c>
-      <c r="E11" s="174">
-        <v>1024</v>
-      </c>
-      <c r="F11" s="174">
-        <v>797</v>
-      </c>
-      <c r="G11" s="174" t="s">
-        <v>1087</v>
-      </c>
-      <c r="H11" s="174"/>
-      <c r="I11" s="174"/>
-      <c r="J11" s="174"/>
-      <c r="K11" s="174"/>
-      <c r="L11" s="174"/>
-      <c r="M11" s="174"/>
-    </row>
-    <row r="12" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="174">
-        <v>35</v>
-      </c>
-      <c r="B12" s="24" t="s">
-        <v>462</v>
-      </c>
-      <c r="C12" s="24" t="s">
-        <v>482</v>
-      </c>
-      <c r="D12" s="176">
-        <v>2</v>
-      </c>
-      <c r="E12" s="174">
-        <v>1024</v>
-      </c>
-      <c r="F12" s="174">
-        <v>794</v>
-      </c>
-      <c r="G12" s="174" t="s">
-        <v>1087</v>
-      </c>
-      <c r="H12" s="174"/>
-      <c r="I12" s="174"/>
-      <c r="J12" s="174"/>
-      <c r="K12" s="174"/>
-      <c r="L12" s="174"/>
-      <c r="M12" s="174"/>
-    </row>
-    <row r="13" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="174">
-        <v>42</v>
-      </c>
-      <c r="B13" s="25" t="s">
-        <v>560</v>
-      </c>
-      <c r="C13" s="174"/>
-      <c r="D13" s="176">
-        <v>2</v>
-      </c>
-      <c r="E13" s="174">
-        <v>1024</v>
-      </c>
-      <c r="F13" s="174">
-        <v>1441</v>
-      </c>
-      <c r="G13" s="174" t="s">
-        <v>1091</v>
-      </c>
-      <c r="H13" s="174"/>
-      <c r="I13" s="174"/>
-      <c r="J13" s="174"/>
-      <c r="K13" s="174"/>
-      <c r="L13" s="174"/>
-      <c r="M13" s="174"/>
-    </row>
-    <row r="14" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="174">
-        <v>43</v>
-      </c>
-      <c r="B14" s="25" t="s">
-        <v>570</v>
-      </c>
-      <c r="C14" s="174"/>
-      <c r="D14" s="176">
-        <v>2</v>
-      </c>
-      <c r="E14" s="174">
-        <v>1024</v>
-      </c>
-      <c r="F14" s="174">
-        <v>1364</v>
-      </c>
-      <c r="G14" s="174" t="s">
-        <v>1091</v>
-      </c>
-      <c r="H14" s="174"/>
-      <c r="I14" s="174"/>
-      <c r="J14" s="174"/>
-      <c r="K14" s="174"/>
-      <c r="L14" s="174"/>
-      <c r="M14" s="174"/>
-    </row>
-    <row r="15" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="174">
-        <v>44</v>
-      </c>
-      <c r="B15" s="85" t="s">
-        <v>577</v>
-      </c>
-      <c r="C15" s="174"/>
-      <c r="D15" s="176">
-        <v>1</v>
-      </c>
-      <c r="E15" s="174">
-        <v>1024</v>
-      </c>
-      <c r="F15" s="174">
-        <v>678</v>
-      </c>
-      <c r="G15" s="174" t="s">
-        <v>1066</v>
-      </c>
-      <c r="H15" s="174">
-        <v>1024</v>
-      </c>
-      <c r="I15" s="174">
-        <v>678</v>
-      </c>
-      <c r="J15" s="174" t="s">
-        <v>1066</v>
-      </c>
-      <c r="K15" s="174"/>
-      <c r="L15" s="174"/>
-      <c r="M15" s="174"/>
-    </row>
-    <row r="16" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="174">
-        <v>45</v>
-      </c>
-      <c r="B16" s="25" t="s">
-        <v>591</v>
-      </c>
-      <c r="C16" s="174"/>
-      <c r="D16" s="176">
-        <v>2</v>
-      </c>
-      <c r="E16" s="174">
-        <v>1024</v>
-      </c>
-      <c r="F16" s="174">
-        <v>1343</v>
-      </c>
-      <c r="G16" s="174" t="s">
-        <v>1092</v>
-      </c>
-      <c r="H16" s="174"/>
-      <c r="I16" s="174"/>
-      <c r="J16" s="174"/>
-      <c r="K16" s="174"/>
-      <c r="L16" s="174"/>
-      <c r="M16" s="174"/>
-    </row>
-    <row r="17" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="174">
-        <v>46</v>
-      </c>
-      <c r="B17" s="25" t="s">
-        <v>599</v>
-      </c>
-      <c r="C17" s="174"/>
-      <c r="D17" s="176">
-        <v>2</v>
-      </c>
-      <c r="E17" s="174">
-        <v>1024</v>
-      </c>
-      <c r="F17" s="174">
-        <v>780</v>
-      </c>
-      <c r="G17" s="174" t="s">
-        <v>1092</v>
-      </c>
-      <c r="H17" s="174"/>
-      <c r="I17" s="174"/>
-      <c r="J17" s="174"/>
-      <c r="K17" s="174"/>
-      <c r="L17" s="174"/>
-      <c r="M17" s="174"/>
-    </row>
-    <row r="18" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="174">
-        <v>47</v>
-      </c>
-      <c r="B18" s="25" t="s">
-        <v>606</v>
-      </c>
-      <c r="C18" s="174"/>
-      <c r="D18" s="176">
-        <v>2</v>
-      </c>
-      <c r="E18" s="174">
-        <v>1024</v>
-      </c>
-      <c r="F18" s="174">
-        <v>881</v>
-      </c>
-      <c r="G18" s="174" t="s">
-        <v>1092</v>
-      </c>
-      <c r="H18" s="174"/>
-      <c r="I18" s="174"/>
-      <c r="J18" s="174"/>
-      <c r="K18" s="174"/>
-      <c r="L18" s="174"/>
-      <c r="M18" s="174"/>
-    </row>
-    <row r="19" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="174">
-        <v>49</v>
-      </c>
-      <c r="B19" s="25" t="s">
-        <v>635</v>
-      </c>
-      <c r="C19" s="174"/>
-      <c r="D19" s="176">
-        <v>1</v>
-      </c>
-      <c r="E19" s="174">
-        <v>1024</v>
-      </c>
-      <c r="F19" s="174">
-        <v>678</v>
-      </c>
-      <c r="G19" s="174" t="s">
-        <v>1066</v>
-      </c>
-      <c r="H19" s="174">
-        <v>1024</v>
-      </c>
-      <c r="I19" s="174">
-        <v>1365</v>
-      </c>
-      <c r="J19" s="174" t="s">
-        <v>1092</v>
-      </c>
-      <c r="K19" s="174"/>
-      <c r="L19" s="174"/>
-      <c r="M19" s="174"/>
-    </row>
-    <row r="20" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="174">
-        <v>53</v>
-      </c>
-      <c r="B20" s="49" t="s">
-        <v>688</v>
-      </c>
-      <c r="C20" s="174"/>
-      <c r="D20" s="176">
-        <v>2</v>
-      </c>
-      <c r="E20" s="174">
-        <v>1024</v>
-      </c>
-      <c r="F20" s="174">
-        <v>796</v>
-      </c>
-      <c r="G20" s="174" t="s">
-        <v>1094</v>
-      </c>
-      <c r="H20" s="174"/>
-      <c r="I20" s="174"/>
-      <c r="J20" s="174"/>
-      <c r="K20" s="174"/>
-      <c r="L20" s="174"/>
-      <c r="M20" s="174"/>
-    </row>
-    <row r="21" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="174">
-        <v>55</v>
-      </c>
-      <c r="B21" s="25" t="s">
-        <v>711</v>
-      </c>
-      <c r="C21" s="174"/>
-      <c r="D21" s="176">
-        <v>1</v>
-      </c>
-      <c r="E21" s="174">
-        <v>1024</v>
-      </c>
-      <c r="F21" s="174">
-        <v>686</v>
-      </c>
-      <c r="G21" s="174" t="s">
-        <v>1066</v>
-      </c>
-      <c r="H21" s="174">
-        <v>1024</v>
-      </c>
-      <c r="I21" s="174">
-        <v>1148</v>
-      </c>
-      <c r="J21" s="174" t="s">
-        <v>1094</v>
-      </c>
-      <c r="K21" s="174"/>
-      <c r="L21" s="174"/>
-      <c r="M21" s="174"/>
-    </row>
-    <row r="22" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="174">
-        <v>57</v>
-      </c>
-      <c r="B22" s="25" t="s">
-        <v>733</v>
-      </c>
-      <c r="C22" s="174"/>
-      <c r="D22" s="176">
-        <v>2</v>
-      </c>
-      <c r="E22" s="174">
-        <v>1024</v>
-      </c>
-      <c r="F22" s="174">
-        <v>1365</v>
-      </c>
-      <c r="G22" s="174" t="s">
-        <v>1092</v>
-      </c>
-      <c r="H22" s="174"/>
-      <c r="I22" s="174"/>
-      <c r="J22" s="174"/>
-      <c r="K22" s="174"/>
-      <c r="L22" s="174"/>
-      <c r="M22" s="174"/>
-    </row>
-    <row r="23" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="174">
-        <v>58</v>
-      </c>
-      <c r="B23" s="25" t="s">
-        <v>743</v>
-      </c>
-      <c r="C23" s="174"/>
-      <c r="D23" s="176">
-        <v>2</v>
-      </c>
-      <c r="E23" s="174">
-        <v>1024</v>
-      </c>
-      <c r="F23" s="174">
-        <v>1212</v>
-      </c>
-      <c r="G23" s="174" t="s">
-        <v>1092</v>
-      </c>
-      <c r="H23" s="174"/>
-      <c r="I23" s="174"/>
-      <c r="J23" s="174"/>
-      <c r="K23" s="174"/>
-      <c r="L23" s="174"/>
-      <c r="M23" s="174"/>
-    </row>
-    <row r="24" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="174">
-        <v>61</v>
-      </c>
-      <c r="B24" s="25" t="s">
-        <v>792</v>
-      </c>
-      <c r="C24" s="174"/>
-      <c r="D24" s="176">
-        <v>1</v>
-      </c>
-      <c r="E24" s="174">
-        <v>1024</v>
-      </c>
-      <c r="F24" s="174">
-        <v>683</v>
-      </c>
-      <c r="G24" s="174" t="s">
-        <v>1066</v>
-      </c>
-      <c r="H24" s="174">
-        <v>1024</v>
-      </c>
-      <c r="I24" s="174">
-        <v>1365</v>
-      </c>
-      <c r="J24" s="174" t="s">
-        <v>1092</v>
-      </c>
-      <c r="K24" s="174"/>
-      <c r="L24" s="174"/>
-      <c r="M24" s="174"/>
-    </row>
-    <row r="25" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="174">
-        <v>62</v>
-      </c>
-      <c r="B25" s="25" t="s">
-        <v>803</v>
-      </c>
-      <c r="C25" s="174"/>
-      <c r="D25" s="176">
-        <v>1</v>
-      </c>
-      <c r="E25" s="174">
-        <v>1024</v>
-      </c>
-      <c r="F25" s="174">
-        <v>686</v>
-      </c>
-      <c r="G25" s="174" t="s">
-        <v>1066</v>
-      </c>
-      <c r="H25" s="174">
-        <v>1024</v>
-      </c>
-      <c r="I25" s="174">
-        <v>1145</v>
-      </c>
-      <c r="J25" s="174" t="s">
-        <v>1094</v>
-      </c>
-      <c r="K25" s="174"/>
-      <c r="L25" s="174"/>
-      <c r="M25" s="174"/>
-    </row>
-    <row r="26" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="174">
-        <v>63</v>
-      </c>
-      <c r="B26" s="25" t="s">
-        <v>815</v>
-      </c>
-      <c r="C26" s="174"/>
-      <c r="D26" s="176">
-        <v>1</v>
-      </c>
-      <c r="E26" s="174">
-        <v>1024</v>
-      </c>
-      <c r="F26" s="174">
-        <v>740</v>
-      </c>
-      <c r="G26" s="174" t="s">
-        <v>1066</v>
-      </c>
-      <c r="H26" s="174">
-        <v>1024</v>
-      </c>
-      <c r="I26" s="174">
-        <v>772</v>
-      </c>
-      <c r="J26" s="174" t="s">
-        <v>1066</v>
-      </c>
-      <c r="K26" s="174"/>
-      <c r="L26" s="174"/>
-      <c r="M26" s="174"/>
-    </row>
-    <row r="27" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="174">
-        <v>65</v>
-      </c>
-      <c r="B27" s="25" t="s">
-        <v>842</v>
-      </c>
-      <c r="C27" s="174"/>
-      <c r="D27" s="176">
-        <v>2</v>
-      </c>
-      <c r="E27" s="174">
-        <v>1024</v>
-      </c>
-      <c r="F27" s="174">
-        <v>795</v>
-      </c>
-      <c r="G27" s="174" t="s">
-        <v>1094</v>
-      </c>
-      <c r="H27" s="174"/>
-      <c r="I27" s="174"/>
-      <c r="J27" s="174"/>
-      <c r="K27" s="174"/>
-      <c r="L27" s="174"/>
-      <c r="M27" s="174"/>
-    </row>
-    <row r="28" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="174">
-        <v>66</v>
-      </c>
-      <c r="B28" s="25" t="s">
-        <v>846</v>
-      </c>
-      <c r="C28" s="174"/>
-      <c r="D28" s="176">
-        <v>2</v>
-      </c>
-      <c r="E28" s="174">
-        <v>1024</v>
-      </c>
-      <c r="F28" s="174">
-        <v>747</v>
-      </c>
-      <c r="G28" s="174" t="s">
-        <v>1094</v>
-      </c>
-      <c r="H28" s="174"/>
-      <c r="I28" s="174"/>
-      <c r="J28" s="174"/>
-      <c r="K28" s="174"/>
-      <c r="L28" s="174"/>
-      <c r="M28" s="174"/>
-    </row>
-    <row r="29" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="174">
-        <v>67</v>
-      </c>
-      <c r="B29" s="25" t="s">
-        <v>850</v>
-      </c>
-      <c r="C29" s="174"/>
-      <c r="D29" s="176">
-        <v>1</v>
-      </c>
-      <c r="E29" s="174">
-        <v>1024</v>
-      </c>
-      <c r="F29" s="174">
-        <v>707</v>
-      </c>
-      <c r="G29" s="174" t="s">
-        <v>1095</v>
-      </c>
-      <c r="H29" s="174">
-        <v>1024</v>
-      </c>
-      <c r="I29" s="174">
-        <v>683</v>
-      </c>
-      <c r="J29" s="174" t="s">
-        <v>1096</v>
-      </c>
-      <c r="K29" s="174"/>
-      <c r="L29" s="174"/>
-      <c r="M29" s="174"/>
-    </row>
-    <row r="30" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="174">
-        <v>69</v>
-      </c>
-      <c r="B30" s="25" t="s">
-        <v>858</v>
-      </c>
-      <c r="C30" s="174"/>
-      <c r="D30" s="176">
-        <v>2</v>
-      </c>
-      <c r="E30" s="174">
-        <v>1024</v>
-      </c>
-      <c r="F30" s="174">
-        <v>1365</v>
-      </c>
-      <c r="G30" s="174" t="s">
-        <v>1092</v>
-      </c>
-      <c r="H30" s="174"/>
-      <c r="I30" s="174"/>
-      <c r="J30" s="174"/>
-      <c r="K30" s="174"/>
-      <c r="L30" s="174"/>
-      <c r="M30" s="174"/>
-    </row>
-    <row r="31" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="174">
-        <v>70</v>
-      </c>
-      <c r="B31" s="25" t="s">
-        <v>864</v>
-      </c>
-      <c r="C31" s="174"/>
-      <c r="D31" s="176">
-        <v>2</v>
-      </c>
-      <c r="E31" s="174">
-        <v>1024</v>
-      </c>
-      <c r="F31" s="174">
-        <v>776</v>
-      </c>
-      <c r="G31" s="174" t="s">
-        <v>1094</v>
-      </c>
-      <c r="H31" s="174"/>
-      <c r="I31" s="174"/>
-      <c r="J31" s="174"/>
-      <c r="K31" s="174"/>
-      <c r="L31" s="174"/>
-      <c r="M31" s="174"/>
-    </row>
-    <row r="32" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A32" s="174">
-        <v>72</v>
-      </c>
-      <c r="B32" s="79" t="s">
-        <v>873</v>
-      </c>
-      <c r="C32" s="174"/>
-      <c r="D32" s="176">
-        <v>2</v>
-      </c>
-      <c r="E32" s="174">
-        <v>1024</v>
-      </c>
-      <c r="F32" s="174">
-        <v>839</v>
-      </c>
-      <c r="G32" s="174" t="s">
-        <v>1098</v>
-      </c>
-      <c r="H32" s="174"/>
-      <c r="I32" s="174"/>
-      <c r="J32" s="174"/>
-      <c r="K32" s="174"/>
-      <c r="L32" s="174"/>
-      <c r="M32" s="174"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
 </file>
</xml_diff>